<commit_message>
draft accumulated phytoplankton data processing
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/tassielakes-data/tassielakes-data/data-governance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/tassie-lake/tassielakes-data/data-governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6E3441-4AB2-7446-9267-205CF1322465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4AB62D-F6D0-C247-902A-A425E2720B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8673,10 +8673,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8999,8 +8995,8 @@
   </sheetPr>
   <dimension ref="A1:F328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="F311" sqref="F311"/>
+    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
+      <selection activeCell="F327" sqref="F327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16330,7 +16326,8 @@
         <v>1070</v>
       </c>
       <c r="F326">
-        <v>4.5999999999999996</v>
+        <f>1/4.6</f>
+        <v>0.21739130434782611</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Upload processed data and header for phytoplankton accumulation
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/tassie-lake/tassielakes-data/data-governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4AB62D-F6D0-C247-902A-A425E2720B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DE4F19-E03C-E946-B4B2-C067C3ECD841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14660" yWindow="-21100" windowWidth="19200" windowHeight="21100" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6555" uniqueCount="2508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6636" uniqueCount="2535">
   <si>
     <t>//</t>
   </si>
@@ -8097,6 +8097,87 @@
   </si>
   <si>
     <t>WQ_GEO_SO4</t>
+  </si>
+  <si>
+    <t>var00767</t>
+  </si>
+  <si>
+    <t>var00768</t>
+  </si>
+  <si>
+    <t>var00769</t>
+  </si>
+  <si>
+    <t>var00770</t>
+  </si>
+  <si>
+    <t>var00771</t>
+  </si>
+  <si>
+    <t>var00772</t>
+  </si>
+  <si>
+    <t>var00773</t>
+  </si>
+  <si>
+    <t>var00774</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHARA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHRYSO</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CRYPTO</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DINO</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_EUGLE</t>
+  </si>
+  <si>
+    <t>var00775</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_OCHRO</t>
+  </si>
+  <si>
+    <t>Bacillariophyta</t>
+  </si>
+  <si>
+    <t>Charophyta</t>
+  </si>
+  <si>
+    <t>Chlorophyta</t>
+  </si>
+  <si>
+    <t>Chrysophyta</t>
+  </si>
+  <si>
+    <t>Cryptophyta</t>
+  </si>
+  <si>
+    <t>Cyanobacteria</t>
+  </si>
+  <si>
+    <t>Dinophyta</t>
+  </si>
+  <si>
+    <t>Euglenophyta</t>
+  </si>
+  <si>
+    <t>Ochrophyta</t>
   </si>
 </sst>
 </file>
@@ -8286,7 +8367,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8364,6 +8445,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8452,7 +8539,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -8654,6 +8741,7 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="1" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8993,10 +9081,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F328"/>
+  <dimension ref="A1:F337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
-      <selection activeCell="F327" sqref="F327"/>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="B338" sqref="B338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16370,7 +16458,188 @@
         <v>96.06</v>
       </c>
     </row>
+    <row r="329" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A329" s="75" t="s">
+        <v>2508</v>
+      </c>
+      <c r="B329" s="6" t="s">
+        <v>2526</v>
+      </c>
+      <c r="C329" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D329" s="6" t="s">
+        <v>2516</v>
+      </c>
+      <c r="E329" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F329" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A330" s="75" t="s">
+        <v>2509</v>
+      </c>
+      <c r="B330" s="6" t="s">
+        <v>2527</v>
+      </c>
+      <c r="C330" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D330" s="6" t="s">
+        <v>2517</v>
+      </c>
+      <c r="E330" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F330" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A331" s="75" t="s">
+        <v>2510</v>
+      </c>
+      <c r="B331" s="6" t="s">
+        <v>2528</v>
+      </c>
+      <c r="C331" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D331" s="6" t="s">
+        <v>2518</v>
+      </c>
+      <c r="E331" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F331" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A332" s="75" t="s">
+        <v>2511</v>
+      </c>
+      <c r="B332" s="6" t="s">
+        <v>2529</v>
+      </c>
+      <c r="C332" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D332" s="6" t="s">
+        <v>2519</v>
+      </c>
+      <c r="E332" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F332" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A333" s="75" t="s">
+        <v>2512</v>
+      </c>
+      <c r="B333" s="6" t="s">
+        <v>2530</v>
+      </c>
+      <c r="C333" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D333" s="6" t="s">
+        <v>2520</v>
+      </c>
+      <c r="E333" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F333" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A334" s="75" t="s">
+        <v>2513</v>
+      </c>
+      <c r="B334" s="6" t="s">
+        <v>2531</v>
+      </c>
+      <c r="C334" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D334" s="6" t="s">
+        <v>2521</v>
+      </c>
+      <c r="E334" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F334" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A335" s="75" t="s">
+        <v>2514</v>
+      </c>
+      <c r="B335" s="6" t="s">
+        <v>2532</v>
+      </c>
+      <c r="C335" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D335" s="6" t="s">
+        <v>2522</v>
+      </c>
+      <c r="E335" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F335" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A336" s="75" t="s">
+        <v>2515</v>
+      </c>
+      <c r="B336" s="6" t="s">
+        <v>2533</v>
+      </c>
+      <c r="C336" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D336" s="6" t="s">
+        <v>2523</v>
+      </c>
+      <c r="E336" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F336" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A337" s="75" t="s">
+        <v>2524</v>
+      </c>
+      <c r="B337" s="6" t="s">
+        <v>2534</v>
+      </c>
+      <c r="C337" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D337" s="6" t="s">
+        <v>2525</v>
+      </c>
+      <c r="E337" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F337" s="5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -19761,11 +20030,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:V546"/>
+  <dimension ref="A1:V555"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A522" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B268" sqref="B268"/>
+      <pane ySplit="1" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B551" sqref="B551"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -32429,6 +32698,132 @@
       </c>
       <c r="K546" s="70" t="s">
         <v>2470</v>
+      </c>
+    </row>
+    <row r="547" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A547" s="69" t="s">
+        <v>2508</v>
+      </c>
+      <c r="B547" s="6" t="s">
+        <v>2526</v>
+      </c>
+      <c r="C547" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="K547" s="70" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="548" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A548" s="69" t="s">
+        <v>2509</v>
+      </c>
+      <c r="B548" s="6" t="s">
+        <v>2527</v>
+      </c>
+      <c r="C548" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="K548" s="70" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="549" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A549" s="69" t="s">
+        <v>2510</v>
+      </c>
+      <c r="B549" s="6" t="s">
+        <v>2528</v>
+      </c>
+      <c r="C549" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="K549" s="70" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="550" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A550" s="69" t="s">
+        <v>2511</v>
+      </c>
+      <c r="B550" s="6" t="s">
+        <v>2529</v>
+      </c>
+      <c r="C550" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="K550" s="70" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="551" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A551" s="69" t="s">
+        <v>2512</v>
+      </c>
+      <c r="B551" s="6" t="s">
+        <v>2530</v>
+      </c>
+      <c r="C551" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="K551" s="70" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="552" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A552" s="69" t="s">
+        <v>2513</v>
+      </c>
+      <c r="B552" s="6" t="s">
+        <v>2531</v>
+      </c>
+      <c r="C552" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="K552" s="70" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="553" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A553" s="69" t="s">
+        <v>2514</v>
+      </c>
+      <c r="B553" s="6" t="s">
+        <v>2532</v>
+      </c>
+      <c r="C553" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="K553" s="70" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="554" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A554" s="69" t="s">
+        <v>2515</v>
+      </c>
+      <c r="B554" s="6" t="s">
+        <v>2533</v>
+      </c>
+      <c r="C554" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="K554" s="70" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="555" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A555" s="6" t="s">
+        <v>2524</v>
+      </c>
+      <c r="B555" s="6" t="s">
+        <v>2534</v>
+      </c>
+      <c r="C555" s="6" t="s">
+        <v>2460</v>
+      </c>
+      <c r="K555" s="70" t="s">
+        <v>1456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extract initial value for variables, format marvl plot, organise plot files
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/tassie-lake/tassielakes-data/data-governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DE4F19-E03C-E946-B4B2-C067C3ECD841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9E10E7-4328-9A46-AC1B-713BBD53C1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14660" yWindow="-21100" windowWidth="19200" windowHeight="21100" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14660" yWindow="-21100" windowWidth="19200" windowHeight="19920" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6636" uniqueCount="2535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6637" uniqueCount="2523">
   <si>
     <t>//</t>
   </si>
@@ -8006,69 +8006,39 @@
     <t>WQ_DIAG_PHY_PHAE</t>
   </si>
   <si>
-    <t>Copper - Total/NonFilt as Cu</t>
-  </si>
-  <si>
     <t>WQ_GEO_TCU</t>
   </si>
   <si>
-    <t>Lead - Total/NonFilt as Pb</t>
-  </si>
-  <si>
     <t>WQ_GEO_TPB</t>
   </si>
   <si>
-    <t>Nickel - Total/NonFilt as Ni</t>
-  </si>
-  <si>
     <t>WQ_GEO_TNI</t>
   </si>
   <si>
-    <t>Zinc - Total/NonFilt as Zn</t>
-  </si>
-  <si>
     <t>WQ_GEO_TZN</t>
   </si>
   <si>
-    <t>Aluminium - Total/NonFilt as Al</t>
-  </si>
-  <si>
     <t>WQ_GEO_TAL</t>
   </si>
   <si>
     <t>WQ_GEO_BALK</t>
   </si>
   <si>
-    <t>Chloride as Cl</t>
-  </si>
-  <si>
     <t>WQ_GEO_CL</t>
   </si>
   <si>
     <t>WQ_PHY_BGA</t>
   </si>
   <si>
-    <t>Iron  - Dissolved/Filt as Fe</t>
-  </si>
-  <si>
     <t>WQ_GEO_FEII</t>
   </si>
   <si>
-    <t>Iron - Total/NonFilt as Fe</t>
-  </si>
-  <si>
     <t>WQ_GEO_TFE</t>
   </si>
   <si>
-    <t>Manganese - Total/NonFilt as Mn</t>
-  </si>
-  <si>
     <t>WQ_GEO_TMN</t>
   </si>
   <si>
-    <t>Mercury - Total as Hg</t>
-  </si>
-  <si>
     <t>WQ_GEO_THG</t>
   </si>
   <si>
@@ -8078,18 +8048,9 @@
     <t>WQ_PTX_MICROCYSTIN_IN</t>
   </si>
   <si>
-    <t>Organic Carbon Non-Purgeable (NPOC Dis)</t>
-  </si>
-  <si>
-    <t>Organic Carbon Non-Purgeable (NPOC Tot)</t>
-  </si>
-  <si>
     <t>WQ_DIAG_OGM_TOC</t>
   </si>
   <si>
-    <t>Oxidised Nitrite + Nitrate - Total as N</t>
-  </si>
-  <si>
     <t>WQ_DIAG_NIT_NOX</t>
   </si>
   <si>
@@ -8178,6 +8139,9 @@
   </si>
   <si>
     <t>Ochrophyta</t>
+  </si>
+  <si>
+    <t>WQ_OGM_DOC_OLD</t>
   </si>
 </sst>
 </file>
@@ -8539,7 +8503,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -8742,6 +8706,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="16" borderId="1" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9081,10 +9048,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F337"/>
+  <dimension ref="A1:F338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
-      <selection activeCell="B338" sqref="B338"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B323" sqref="B323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9761,8 +9728,8 @@
         <f>VLOOKUP(A29,'MASTER KEY'!$A$2:$C987,3,TRUE)</f>
         <v>mg/L</v>
       </c>
-      <c r="D29" s="36" t="s">
-        <v>1031</v>
+      <c r="D29" s="76" t="s">
+        <v>2522</v>
       </c>
       <c r="E29" s="27" t="s">
         <v>1002</v>
@@ -16062,13 +16029,13 @@
         <v>920</v>
       </c>
       <c r="B309" t="s">
-        <v>2477</v>
+        <v>919</v>
       </c>
       <c r="C309" s="6" t="s">
         <v>2458</v>
       </c>
       <c r="D309" s="5" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
       <c r="E309" t="s">
         <v>1002</v>
@@ -16082,13 +16049,13 @@
         <v>923</v>
       </c>
       <c r="B310" t="s">
-        <v>2479</v>
+        <v>922</v>
       </c>
       <c r="C310" s="6" t="s">
         <v>2458</v>
       </c>
       <c r="D310" s="5" t="s">
-        <v>2480</v>
+        <v>2478</v>
       </c>
       <c r="E310" t="s">
         <v>1002</v>
@@ -16102,13 +16069,13 @@
         <v>925</v>
       </c>
       <c r="B311" t="s">
-        <v>2481</v>
+        <v>924</v>
       </c>
       <c r="C311" s="6" t="s">
         <v>2458</v>
       </c>
       <c r="D311" s="5" t="s">
-        <v>2482</v>
+        <v>2479</v>
       </c>
       <c r="E311" t="s">
         <v>1002</v>
@@ -16122,13 +16089,13 @@
         <v>929</v>
       </c>
       <c r="B312" t="s">
-        <v>2483</v>
+        <v>928</v>
       </c>
       <c r="C312" s="6" t="s">
         <v>2458</v>
       </c>
       <c r="D312" s="5" t="s">
-        <v>2484</v>
+        <v>2480</v>
       </c>
       <c r="E312" t="s">
         <v>1002</v>
@@ -16142,13 +16109,13 @@
         <v>2139</v>
       </c>
       <c r="B313" t="s">
-        <v>2485</v>
+        <v>2140</v>
       </c>
       <c r="C313" s="6" t="s">
         <v>2458</v>
       </c>
       <c r="D313" s="5" t="s">
-        <v>2486</v>
+        <v>2481</v>
       </c>
       <c r="E313" t="s">
         <v>1002</v>
@@ -16168,7 +16135,7 @@
         <v>2458</v>
       </c>
       <c r="D314" s="5" t="s">
-        <v>2487</v>
+        <v>2482</v>
       </c>
       <c r="E314" t="s">
         <v>1002</v>
@@ -16182,13 +16149,13 @@
         <v>2193</v>
       </c>
       <c r="B315" t="s">
-        <v>2488</v>
+        <v>2194</v>
       </c>
       <c r="C315" s="6" t="s">
         <v>2458</v>
       </c>
       <c r="D315" s="5" t="s">
-        <v>2489</v>
+        <v>2483</v>
       </c>
       <c r="E315" t="s">
         <v>1002</v>
@@ -16208,7 +16175,7 @@
         <v>2460</v>
       </c>
       <c r="D316" s="5" t="s">
-        <v>2490</v>
+        <v>2484</v>
       </c>
       <c r="E316" t="s">
         <v>1002</v>
@@ -16222,13 +16189,13 @@
         <v>2371</v>
       </c>
       <c r="B317" t="s">
-        <v>2491</v>
+        <v>2372</v>
       </c>
       <c r="C317" s="6" t="s">
         <v>2458</v>
       </c>
       <c r="D317" s="5" t="s">
-        <v>2492</v>
+        <v>2485</v>
       </c>
       <c r="E317" t="s">
         <v>1002</v>
@@ -16242,13 +16209,13 @@
         <v>2373</v>
       </c>
       <c r="B318" t="s">
-        <v>2493</v>
+        <v>2374</v>
       </c>
       <c r="C318" s="6" t="s">
         <v>2458</v>
       </c>
       <c r="D318" s="5" t="s">
-        <v>2494</v>
+        <v>2486</v>
       </c>
       <c r="E318" t="s">
         <v>1002</v>
@@ -16262,13 +16229,13 @@
         <v>2375</v>
       </c>
       <c r="B319" t="s">
-        <v>2495</v>
+        <v>2376</v>
       </c>
       <c r="C319" s="6" t="s">
         <v>2458</v>
       </c>
       <c r="D319" s="5" t="s">
-        <v>2496</v>
+        <v>2487</v>
       </c>
       <c r="E319" t="s">
         <v>1002</v>
@@ -16282,13 +16249,13 @@
         <v>2377</v>
       </c>
       <c r="B320" t="s">
-        <v>2497</v>
+        <v>2378</v>
       </c>
       <c r="C320" s="6" t="s">
         <v>2458</v>
       </c>
       <c r="D320" s="5" t="s">
-        <v>2498</v>
+        <v>2488</v>
       </c>
       <c r="E320" t="s">
         <v>1002</v>
@@ -16308,7 +16275,7 @@
         <v>2464</v>
       </c>
       <c r="D321" s="5" t="s">
-        <v>2499</v>
+        <v>2489</v>
       </c>
       <c r="E321" t="s">
         <v>1002</v>
@@ -16328,7 +16295,7 @@
         <v>2464</v>
       </c>
       <c r="D322" s="5" t="s">
-        <v>2500</v>
+        <v>2490</v>
       </c>
       <c r="E322" t="s">
         <v>1002</v>
@@ -16342,7 +16309,7 @@
         <v>2408</v>
       </c>
       <c r="B323" t="s">
-        <v>2501</v>
+        <v>2409</v>
       </c>
       <c r="C323" s="6" t="s">
         <v>2458</v>
@@ -16362,13 +16329,13 @@
         <v>2410</v>
       </c>
       <c r="B324" t="s">
-        <v>2502</v>
+        <v>2411</v>
       </c>
       <c r="C324" s="6" t="s">
         <v>2458</v>
       </c>
       <c r="D324" s="5" t="s">
-        <v>2503</v>
+        <v>2491</v>
       </c>
       <c r="E324" t="s">
         <v>1002</v>
@@ -16382,13 +16349,13 @@
         <v>2412</v>
       </c>
       <c r="B325" t="s">
-        <v>2504</v>
+        <v>2413</v>
       </c>
       <c r="C325" s="6" t="s">
         <v>921</v>
       </c>
       <c r="D325" s="5" t="s">
-        <v>2505</v>
+        <v>2492</v>
       </c>
       <c r="E325" t="s">
         <v>1002</v>
@@ -16429,7 +16396,7 @@
         <v>2458</v>
       </c>
       <c r="D327" s="6" t="s">
-        <v>2506</v>
+        <v>2493</v>
       </c>
       <c r="E327" s="6" t="s">
         <v>1002</v>
@@ -16449,7 +16416,7 @@
         <v>2458</v>
       </c>
       <c r="D328" s="6" t="s">
-        <v>2507</v>
+        <v>2494</v>
       </c>
       <c r="E328" s="6" t="s">
         <v>1002</v>
@@ -16460,16 +16427,16 @@
     </row>
     <row r="329" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A329" s="75" t="s">
-        <v>2508</v>
+        <v>2495</v>
       </c>
       <c r="B329" s="6" t="s">
-        <v>2526</v>
+        <v>2513</v>
       </c>
       <c r="C329" s="69" t="s">
         <v>2460</v>
       </c>
       <c r="D329" s="6" t="s">
-        <v>2516</v>
+        <v>2503</v>
       </c>
       <c r="E329" s="69" t="s">
         <v>2460</v>
@@ -16480,16 +16447,16 @@
     </row>
     <row r="330" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A330" s="75" t="s">
-        <v>2509</v>
+        <v>2496</v>
       </c>
       <c r="B330" s="6" t="s">
-        <v>2527</v>
+        <v>2514</v>
       </c>
       <c r="C330" s="69" t="s">
         <v>2460</v>
       </c>
       <c r="D330" s="6" t="s">
-        <v>2517</v>
+        <v>2504</v>
       </c>
       <c r="E330" s="69" t="s">
         <v>2460</v>
@@ -16500,16 +16467,16 @@
     </row>
     <row r="331" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A331" s="75" t="s">
-        <v>2510</v>
+        <v>2497</v>
       </c>
       <c r="B331" s="6" t="s">
-        <v>2528</v>
+        <v>2515</v>
       </c>
       <c r="C331" s="69" t="s">
         <v>2460</v>
       </c>
       <c r="D331" s="6" t="s">
-        <v>2518</v>
+        <v>2505</v>
       </c>
       <c r="E331" s="69" t="s">
         <v>2460</v>
@@ -16520,16 +16487,16 @@
     </row>
     <row r="332" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A332" s="75" t="s">
-        <v>2511</v>
+        <v>2498</v>
       </c>
       <c r="B332" s="6" t="s">
-        <v>2529</v>
+        <v>2516</v>
       </c>
       <c r="C332" s="69" t="s">
         <v>2460</v>
       </c>
       <c r="D332" s="6" t="s">
-        <v>2519</v>
+        <v>2506</v>
       </c>
       <c r="E332" s="69" t="s">
         <v>2460</v>
@@ -16540,16 +16507,16 @@
     </row>
     <row r="333" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A333" s="75" t="s">
-        <v>2512</v>
+        <v>2499</v>
       </c>
       <c r="B333" s="6" t="s">
-        <v>2530</v>
+        <v>2517</v>
       </c>
       <c r="C333" s="69" t="s">
         <v>2460</v>
       </c>
       <c r="D333" s="6" t="s">
-        <v>2520</v>
+        <v>2507</v>
       </c>
       <c r="E333" s="69" t="s">
         <v>2460</v>
@@ -16560,16 +16527,16 @@
     </row>
     <row r="334" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A334" s="75" t="s">
-        <v>2513</v>
+        <v>2500</v>
       </c>
       <c r="B334" s="6" t="s">
-        <v>2531</v>
+        <v>2518</v>
       </c>
       <c r="C334" s="69" t="s">
         <v>2460</v>
       </c>
       <c r="D334" s="6" t="s">
-        <v>2521</v>
+        <v>2508</v>
       </c>
       <c r="E334" s="69" t="s">
         <v>2460</v>
@@ -16580,16 +16547,16 @@
     </row>
     <row r="335" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A335" s="75" t="s">
-        <v>2514</v>
+        <v>2501</v>
       </c>
       <c r="B335" s="6" t="s">
-        <v>2532</v>
+        <v>2519</v>
       </c>
       <c r="C335" s="69" t="s">
         <v>2460</v>
       </c>
       <c r="D335" s="6" t="s">
-        <v>2522</v>
+        <v>2509</v>
       </c>
       <c r="E335" s="69" t="s">
         <v>2460</v>
@@ -16600,16 +16567,16 @@
     </row>
     <row r="336" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A336" s="75" t="s">
-        <v>2515</v>
+        <v>2502</v>
       </c>
       <c r="B336" s="6" t="s">
-        <v>2533</v>
+        <v>2520</v>
       </c>
       <c r="C336" s="69" t="s">
         <v>2460</v>
       </c>
       <c r="D336" s="6" t="s">
-        <v>2523</v>
+        <v>2510</v>
       </c>
       <c r="E336" s="69" t="s">
         <v>2460</v>
@@ -16620,22 +16587,27 @@
     </row>
     <row r="337" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A337" s="75" t="s">
-        <v>2524</v>
+        <v>2511</v>
       </c>
       <c r="B337" s="6" t="s">
-        <v>2534</v>
+        <v>2521</v>
       </c>
       <c r="C337" s="69" t="s">
         <v>2460</v>
       </c>
       <c r="D337" s="6" t="s">
-        <v>2525</v>
+        <v>2512</v>
       </c>
       <c r="E337" s="69" t="s">
         <v>2460</v>
       </c>
       <c r="F337" s="5">
         <v>1</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B338" s="6" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -20032,9 +20004,9 @@
   </sheetPr>
   <dimension ref="A1:V555"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B551" sqref="B551"/>
+    <sheetView topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -32702,10 +32674,10 @@
     </row>
     <row r="547" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A547" s="69" t="s">
-        <v>2508</v>
+        <v>2495</v>
       </c>
       <c r="B547" s="6" t="s">
-        <v>2526</v>
+        <v>2513</v>
       </c>
       <c r="C547" s="69" t="s">
         <v>2460</v>
@@ -32716,10 +32688,10 @@
     </row>
     <row r="548" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A548" s="69" t="s">
-        <v>2509</v>
+        <v>2496</v>
       </c>
       <c r="B548" s="6" t="s">
-        <v>2527</v>
+        <v>2514</v>
       </c>
       <c r="C548" s="69" t="s">
         <v>2460</v>
@@ -32730,10 +32702,10 @@
     </row>
     <row r="549" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A549" s="69" t="s">
-        <v>2510</v>
+        <v>2497</v>
       </c>
       <c r="B549" s="6" t="s">
-        <v>2528</v>
+        <v>2515</v>
       </c>
       <c r="C549" s="69" t="s">
         <v>2460</v>
@@ -32744,10 +32716,10 @@
     </row>
     <row r="550" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A550" s="69" t="s">
-        <v>2511</v>
+        <v>2498</v>
       </c>
       <c r="B550" s="6" t="s">
-        <v>2529</v>
+        <v>2516</v>
       </c>
       <c r="C550" s="69" t="s">
         <v>2460</v>
@@ -32758,10 +32730,10 @@
     </row>
     <row r="551" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A551" s="69" t="s">
-        <v>2512</v>
+        <v>2499</v>
       </c>
       <c r="B551" s="6" t="s">
-        <v>2530</v>
+        <v>2517</v>
       </c>
       <c r="C551" s="69" t="s">
         <v>2460</v>
@@ -32772,10 +32744,10 @@
     </row>
     <row r="552" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A552" s="69" t="s">
-        <v>2513</v>
+        <v>2500</v>
       </c>
       <c r="B552" s="6" t="s">
-        <v>2531</v>
+        <v>2518</v>
       </c>
       <c r="C552" s="69" t="s">
         <v>2460</v>
@@ -32786,10 +32758,10 @@
     </row>
     <row r="553" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A553" s="69" t="s">
-        <v>2514</v>
+        <v>2501</v>
       </c>
       <c r="B553" s="6" t="s">
-        <v>2532</v>
+        <v>2519</v>
       </c>
       <c r="C553" s="69" t="s">
         <v>2460</v>
@@ -32800,10 +32772,10 @@
     </row>
     <row r="554" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A554" s="69" t="s">
-        <v>2515</v>
+        <v>2502</v>
       </c>
       <c r="B554" s="6" t="s">
-        <v>2533</v>
+        <v>2520</v>
       </c>
       <c r="C554" s="69" t="s">
         <v>2460</v>
@@ -32814,10 +32786,10 @@
     </row>
     <row r="555" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A555" s="6" t="s">
-        <v>2524</v>
+        <v>2511</v>
       </c>
       <c r="B555" s="6" t="s">
-        <v>2534</v>
+        <v>2521</v>
       </c>
       <c r="C555" s="6" t="s">
         <v>2460</v>

</xml_diff>

<commit_message>
Check and update variable key conversion factor
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/tassie-lake/tassielakes-data/data-governance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/updates/tassielakes-data/data-governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C904E70F-12EB-A540-87D2-CD3B91E3A3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFA11DE-FBE4-C447-956D-18B73C73CC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,7 +434,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6637" uniqueCount="2523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6637" uniqueCount="2524">
   <si>
     <t>//</t>
   </si>
@@ -8130,11 +8130,17 @@
   <si>
     <t>SECCHI_DEPTH</t>
   </si>
+  <si>
+    <t>WQ_DIAG_TOT_PAR_OLD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -8325,7 +8331,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8409,6 +8415,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8497,7 +8509,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -8704,6 +8716,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9043,10 +9060,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F338"/>
+  <dimension ref="A1:G338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="F329" sqref="F329"/>
+    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="F257" sqref="F257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9059,7 +9076,7 @@
     <col min="6" max="6" width="9.5" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>990</v>
       </c>
@@ -9079,7 +9096,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="str">
         <f>'MASTER KEY'!A2</f>
         <v>var00001</v>
@@ -9101,8 +9118,9 @@
       <c r="F2" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G2" s="79"/>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="str">
         <f>'MASTER KEY'!A3</f>
         <v>var00002</v>
@@ -9124,8 +9142,9 @@
       <c r="F3" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="79"/>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="str">
         <f>'MASTER KEY'!A4</f>
         <v>var00003</v>
@@ -9144,11 +9163,12 @@
       <c r="E4" s="27" t="s">
         <v>1000</v>
       </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="78">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="79"/>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="str">
         <f>'MASTER KEY'!A5</f>
         <v>var00004</v>
@@ -9171,8 +9191,9 @@
         <f>1000/14</f>
         <v>71.428571428571431</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="79"/>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="str">
         <f>'MASTER KEY'!A6</f>
         <v>var00005</v>
@@ -9195,8 +9216,9 @@
         <f>1000/31</f>
         <v>32.258064516129032</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G6" s="79"/>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="71" t="str">
         <f>'MASTER KEY'!A7</f>
         <v>var00006</v>
@@ -9218,8 +9240,9 @@
       <c r="F7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G7" s="79"/>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="71" t="str">
         <f>'MASTER KEY'!A8</f>
         <v>var00007</v>
@@ -9241,8 +9264,9 @@
       <c r="F8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G8" s="79"/>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="str">
         <f>'MASTER KEY'!A9</f>
         <v>var00008</v>
@@ -9264,8 +9288,9 @@
       <c r="F9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G9" s="79"/>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="71" t="str">
         <f>'MASTER KEY'!A10</f>
         <v>var00009</v>
@@ -9288,8 +9313,9 @@
         <f>1000/14</f>
         <v>71.428571428571431</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G10" s="79"/>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="71" t="str">
         <f>'MASTER KEY'!A11</f>
         <v>var00010</v>
@@ -9312,8 +9338,9 @@
         <f>1000/31</f>
         <v>32.258064516129032</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G11" s="79"/>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="str">
         <f>'MASTER KEY'!A12</f>
         <v>var00011</v>
@@ -9336,8 +9363,9 @@
         <f>1000/12</f>
         <v>83.333333333333329</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G12" s="79"/>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="71" t="str">
         <f>'MASTER KEY'!A13</f>
         <v>var00012</v>
@@ -9359,8 +9387,9 @@
       <c r="F13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G13" s="79"/>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="71" t="str">
         <f>'MASTER KEY'!A14</f>
         <v>var00013</v>
@@ -9382,8 +9411,9 @@
       <c r="F14" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G14" s="79"/>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="71" t="str">
         <f>'MASTER KEY'!A15</f>
         <v>var00014</v>
@@ -9405,8 +9435,9 @@
       <c r="F15" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G15" s="79"/>
+    </row>
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="str">
         <f>'MASTER KEY'!A16</f>
         <v>var00016</v>
@@ -9428,8 +9459,9 @@
       <c r="F16" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G16" s="79"/>
+    </row>
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="str">
         <f>'MASTER KEY'!A17</f>
         <v>var00017</v>
@@ -9451,8 +9483,9 @@
       <c r="F17" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G17" s="79"/>
+    </row>
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="str">
         <f>'MASTER KEY'!A18</f>
         <v>var00018</v>
@@ -9474,8 +9507,9 @@
       <c r="F18" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G18" s="79"/>
+    </row>
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="str">
         <f>'MASTER KEY'!A19</f>
         <v>var00019</v>
@@ -9497,8 +9531,9 @@
       <c r="F19" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G19" s="79"/>
+    </row>
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="str">
         <f>'MASTER KEY'!A20</f>
         <v>var00020</v>
@@ -9520,8 +9555,9 @@
       <c r="F20" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G20" s="79"/>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="str">
         <f>'MASTER KEY'!A21</f>
         <v>var00021</v>
@@ -9543,8 +9579,9 @@
       <c r="F21" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G21" s="79"/>
+    </row>
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="str">
         <f>'MASTER KEY'!A22</f>
         <v>var00022</v>
@@ -9566,8 +9603,9 @@
       <c r="F22" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G22" s="80"/>
+    </row>
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="71" t="str">
         <f>'MASTER KEY'!A23</f>
         <v>var00023</v>
@@ -9590,8 +9628,9 @@
         <f>1000/32</f>
         <v>31.25</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G23" s="79"/>
+    </row>
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="str">
         <f>'MASTER KEY'!A24</f>
         <v>var00024</v>
@@ -9613,8 +9652,9 @@
       <c r="F24" s="14">
         <v>35.587188609999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G24" s="79"/>
+    </row>
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="71" t="str">
         <f>'MASTER KEY'!A25</f>
         <v>var00025</v>
@@ -9637,8 +9677,9 @@
         <f>1000/14</f>
         <v>71.428571428571431</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G25" s="79"/>
+    </row>
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="71" t="str">
         <f>'MASTER KEY'!A26</f>
         <v>var00026</v>
@@ -9661,8 +9702,9 @@
         <f>1000/14</f>
         <v>71.428571428571431</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G26" s="79"/>
+    </row>
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="71" t="str">
         <f>'MASTER KEY'!A27</f>
         <v>var00027</v>
@@ -9685,8 +9727,9 @@
         <f>1000/31</f>
         <v>32.258064516129032</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G27" s="79"/>
+    </row>
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="str">
         <f>'MASTER KEY'!A28</f>
         <v>var00028</v>
@@ -9709,8 +9752,9 @@
         <f>1000/31</f>
         <v>32.258064516129032</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G28" s="79"/>
+    </row>
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27" t="str">
         <f>'MASTER KEY'!A29</f>
         <v>var00029</v>
@@ -9733,8 +9777,9 @@
         <f>1000/12</f>
         <v>83.333333333333329</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G29" s="79"/>
+    </row>
+    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="27" t="str">
         <f>'MASTER KEY'!A30</f>
         <v>var00030</v>
@@ -9757,8 +9802,9 @@
         <f>1000/12</f>
         <v>83.333333333333329</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G30" s="79"/>
+    </row>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="27" t="str">
         <f>'MASTER KEY'!A31</f>
         <v>var00031</v>
@@ -9781,8 +9827,9 @@
         <f>1000/12</f>
         <v>83.333333333333329</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G31" s="79"/>
+    </row>
+    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="27" t="str">
         <f>'MASTER KEY'!A32</f>
         <v>var00032</v>
@@ -9805,8 +9852,9 @@
         <f>1000/14</f>
         <v>71.428571428571431</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G32" s="79"/>
+    </row>
+    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="27" t="str">
         <f>'MASTER KEY'!A33</f>
         <v>var00033</v>
@@ -9829,8 +9877,9 @@
         <f>1000/14</f>
         <v>71.428571428571431</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G33" s="79"/>
+    </row>
+    <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="27" t="str">
         <f>'MASTER KEY'!A34</f>
         <v>var00034</v>
@@ -9853,8 +9902,9 @@
         <f>1000/14</f>
         <v>71.428571428571431</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G34" s="79"/>
+    </row>
+    <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="27" t="str">
         <f>'MASTER KEY'!A35</f>
         <v>var00035</v>
@@ -9877,8 +9927,9 @@
         <f>1000/31</f>
         <v>32.258064516129032</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G35" s="79"/>
+    </row>
+    <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="27" t="str">
         <f>'MASTER KEY'!A36</f>
         <v>var00036</v>
@@ -9901,8 +9952,9 @@
         <f>1000/31</f>
         <v>32.258064516129032</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G36" s="79"/>
+    </row>
+    <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="str">
         <f>'MASTER KEY'!A37</f>
         <v>var00037</v>
@@ -9925,8 +9977,9 @@
         <f>1000/31</f>
         <v>32.258064516129032</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G37" s="79"/>
+    </row>
+    <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="27" t="str">
         <f>'MASTER KEY'!A38</f>
         <v>var00038</v>
@@ -9948,8 +10001,9 @@
       <c r="F38" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G38" s="79"/>
+    </row>
+    <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="27" t="str">
         <f>'MASTER KEY'!A39</f>
         <v>var00039</v>
@@ -9971,8 +10025,9 @@
       <c r="F39" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G39" s="79"/>
+    </row>
+    <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="27" t="str">
         <f>'MASTER KEY'!A40</f>
         <v>var00040</v>
@@ -9994,8 +10049,9 @@
       <c r="F40" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G40" s="79"/>
+    </row>
+    <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="27" t="str">
         <f>'MASTER KEY'!A41</f>
         <v>var00041</v>
@@ -10017,8 +10073,9 @@
       <c r="F41" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G41" s="79"/>
+    </row>
+    <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="27" t="str">
         <f>'MASTER KEY'!A42</f>
         <v>var00042</v>
@@ -10040,8 +10097,9 @@
       <c r="F42" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G42" s="79"/>
+    </row>
+    <row r="43" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="27" t="str">
         <f>'MASTER KEY'!A43</f>
         <v>var00043</v>
@@ -10063,8 +10121,9 @@
       <c r="F43" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G43" s="79"/>
+    </row>
+    <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="27" t="str">
         <f>'MASTER KEY'!A44</f>
         <v>var00044</v>
@@ -10086,8 +10145,9 @@
       <c r="F44" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G44" s="79"/>
+    </row>
+    <row r="45" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="27" t="str">
         <f>'MASTER KEY'!A45</f>
         <v>var00045</v>
@@ -10109,8 +10169,9 @@
       <c r="F45" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G45" s="79"/>
+    </row>
+    <row r="46" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="27" t="str">
         <f>'MASTER KEY'!A46</f>
         <v>var00046</v>
@@ -10132,8 +10193,9 @@
       <c r="F46" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G46" s="79"/>
+    </row>
+    <row r="47" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="27" t="str">
         <f>'MASTER KEY'!A47</f>
         <v>var00047</v>
@@ -10155,8 +10217,9 @@
       <c r="F47" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G47" s="79"/>
+    </row>
+    <row r="48" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="27" t="str">
         <f>'MASTER KEY'!A48</f>
         <v>var00048</v>
@@ -10178,8 +10241,9 @@
       <c r="F48" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G48" s="79"/>
+    </row>
+    <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="27" t="str">
         <f>'MASTER KEY'!A49</f>
         <v>var00049</v>
@@ -10201,8 +10265,9 @@
       <c r="F49" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G49" s="79"/>
+    </row>
+    <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="27" t="str">
         <f>'MASTER KEY'!A50</f>
         <v>var00050</v>
@@ -10224,8 +10289,9 @@
       <c r="F50" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G50" s="79"/>
+    </row>
+    <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="27" t="str">
         <f>'MASTER KEY'!A51</f>
         <v>var00051</v>
@@ -10247,8 +10313,9 @@
       <c r="F51" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G51" s="79"/>
+    </row>
+    <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="27" t="str">
         <f>'MASTER KEY'!A52</f>
         <v>var00052</v>
@@ -10270,8 +10337,9 @@
       <c r="F52" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G52" s="79"/>
+    </row>
+    <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="27" t="str">
         <f>'MASTER KEY'!A53</f>
         <v>var00053</v>
@@ -10293,8 +10361,9 @@
       <c r="F53" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G53" s="79"/>
+    </row>
+    <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="27" t="str">
         <f>'MASTER KEY'!A54</f>
         <v>var00054</v>
@@ -10316,8 +10385,9 @@
       <c r="F54" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G54" s="79"/>
+    </row>
+    <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="27" t="str">
         <f>'MASTER KEY'!A55</f>
         <v>var00055</v>
@@ -10339,8 +10409,9 @@
       <c r="F55" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G55" s="79"/>
+    </row>
+    <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="27" t="str">
         <f>'MASTER KEY'!A56</f>
         <v>var00056</v>
@@ -10362,8 +10433,9 @@
       <c r="F56" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G56" s="79"/>
+    </row>
+    <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="27" t="str">
         <f>'MASTER KEY'!A57</f>
         <v>var00057</v>
@@ -10385,8 +10457,9 @@
       <c r="F57" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G57" s="79"/>
+    </row>
+    <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="27" t="str">
         <f>'MASTER KEY'!A58</f>
         <v>var00058</v>
@@ -10408,8 +10481,9 @@
       <c r="F58" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G58" s="79"/>
+    </row>
+    <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="27" t="str">
         <f>'MASTER KEY'!A59</f>
         <v>var00059</v>
@@ -10431,8 +10505,9 @@
       <c r="F59" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G59" s="79"/>
+    </row>
+    <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="27" t="str">
         <f>'MASTER KEY'!A60</f>
         <v>var00060</v>
@@ -10454,8 +10529,9 @@
       <c r="F60" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G60" s="79"/>
+    </row>
+    <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="27" t="str">
         <f>'MASTER KEY'!A61</f>
         <v>var00061</v>
@@ -10477,8 +10553,9 @@
       <c r="F61" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G61" s="79"/>
+    </row>
+    <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="str">
         <f>'MASTER KEY'!A62</f>
         <v>var00062</v>
@@ -10500,8 +10577,9 @@
       <c r="F62" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G62" s="79"/>
+    </row>
+    <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="27" t="str">
         <f>'MASTER KEY'!A63</f>
         <v>var00063</v>
@@ -10523,8 +10601,9 @@
       <c r="F63" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G63" s="79"/>
+    </row>
+    <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="27" t="str">
         <f>'MASTER KEY'!A64</f>
         <v>var00064</v>
@@ -10546,8 +10625,9 @@
       <c r="F64" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G64" s="79"/>
+    </row>
+    <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="27" t="str">
         <f>'MASTER KEY'!A65</f>
         <v>var00065</v>
@@ -10569,8 +10649,9 @@
       <c r="F65" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G65" s="79"/>
+    </row>
+    <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="27" t="str">
         <f>'MASTER KEY'!A66</f>
         <v>var00066</v>
@@ -10592,8 +10673,9 @@
       <c r="F66" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G66" s="79"/>
+    </row>
+    <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="27" t="str">
         <f>'MASTER KEY'!A67</f>
         <v>var00067</v>
@@ -10615,8 +10697,9 @@
       <c r="F67" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G67" s="79"/>
+    </row>
+    <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="27" t="str">
         <f>'MASTER KEY'!A68</f>
         <v>var00068</v>
@@ -10638,8 +10721,9 @@
       <c r="F68" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G68" s="79"/>
+    </row>
+    <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="27" t="str">
         <f>'MASTER KEY'!A69</f>
         <v>var00069</v>
@@ -10661,8 +10745,9 @@
       <c r="F69" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G69" s="79"/>
+    </row>
+    <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="27" t="str">
         <f>'MASTER KEY'!A70</f>
         <v>var00070</v>
@@ -10684,8 +10769,9 @@
       <c r="F70" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G70" s="79"/>
+    </row>
+    <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="27" t="str">
         <f>'MASTER KEY'!A71</f>
         <v>var00071</v>
@@ -10707,8 +10793,9 @@
       <c r="F71" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G71" s="79"/>
+    </row>
+    <row r="72" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="27" t="str">
         <f>'MASTER KEY'!A72</f>
         <v>var00072</v>
@@ -10730,8 +10817,9 @@
       <c r="F72" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G72" s="79"/>
+    </row>
+    <row r="73" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="27" t="str">
         <f>'MASTER KEY'!A73</f>
         <v>var00073</v>
@@ -10753,8 +10841,9 @@
       <c r="F73" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G73" s="79"/>
+    </row>
+    <row r="74" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="27" t="str">
         <f>'MASTER KEY'!A74</f>
         <v>var00074</v>
@@ -10776,8 +10865,9 @@
       <c r="F74" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G74" s="79"/>
+    </row>
+    <row r="75" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="27" t="str">
         <f>'MASTER KEY'!A75</f>
         <v>var00075</v>
@@ -10799,8 +10889,9 @@
       <c r="F75" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G75" s="79"/>
+    </row>
+    <row r="76" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="27" t="str">
         <f>'MASTER KEY'!A76</f>
         <v>var00076</v>
@@ -10822,8 +10913,9 @@
       <c r="F76" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G76" s="79"/>
+    </row>
+    <row r="77" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="27" t="str">
         <f>'MASTER KEY'!A77</f>
         <v>var00077</v>
@@ -10845,8 +10937,9 @@
       <c r="F77" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G77" s="79"/>
+    </row>
+    <row r="78" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="27" t="str">
         <f>'MASTER KEY'!A78</f>
         <v>var00078</v>
@@ -10868,8 +10961,9 @@
       <c r="F78" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G78" s="79"/>
+    </row>
+    <row r="79" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="27" t="str">
         <f>'MASTER KEY'!A79</f>
         <v>var00079</v>
@@ -10891,8 +10985,9 @@
       <c r="F79" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G79" s="79"/>
+    </row>
+    <row r="80" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="27" t="str">
         <f>'MASTER KEY'!A80</f>
         <v>var00080</v>
@@ -10914,8 +11009,9 @@
       <c r="F80" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G80" s="79"/>
+    </row>
+    <row r="81" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="27" t="str">
         <f>'MASTER KEY'!A81</f>
         <v>var00081</v>
@@ -10937,8 +11033,9 @@
       <c r="F81" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G81" s="79"/>
+    </row>
+    <row r="82" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="27" t="str">
         <f>'MASTER KEY'!A82</f>
         <v>var00082</v>
@@ -10960,8 +11057,9 @@
       <c r="F82" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G82" s="79"/>
+    </row>
+    <row r="83" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="27" t="str">
         <f>'MASTER KEY'!A83</f>
         <v>var00083</v>
@@ -10983,8 +11081,9 @@
       <c r="F83" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G83" s="79"/>
+    </row>
+    <row r="84" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="27" t="str">
         <f>'MASTER KEY'!A84</f>
         <v>var00084</v>
@@ -11006,8 +11105,9 @@
       <c r="F84" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G84" s="79"/>
+    </row>
+    <row r="85" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="71" t="str">
         <f>'MASTER KEY'!A85</f>
         <v>var00085</v>
@@ -11029,8 +11129,9 @@
       <c r="F85" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G85" s="79"/>
+    </row>
+    <row r="86" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="27" t="str">
         <f>'MASTER KEY'!A86</f>
         <v>var00087</v>
@@ -11052,8 +11153,9 @@
       <c r="F86" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G86" s="79"/>
+    </row>
+    <row r="87" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="27" t="str">
         <f>'MASTER KEY'!A87</f>
         <v>var00088</v>
@@ -11075,8 +11177,9 @@
       <c r="F87" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G87" s="79"/>
+    </row>
+    <row r="88" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="27" t="str">
         <f>'MASTER KEY'!A88</f>
         <v>var00089</v>
@@ -11098,8 +11201,9 @@
       <c r="F88" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G88" s="79"/>
+    </row>
+    <row r="89" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="27" t="str">
         <f>'MASTER KEY'!A89</f>
         <v>var00090</v>
@@ -11121,8 +11225,9 @@
       <c r="F89" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G89" s="79"/>
+    </row>
+    <row r="90" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="27" t="str">
         <f>'MASTER KEY'!A90</f>
         <v>var00093</v>
@@ -11144,8 +11249,9 @@
       <c r="F90" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G90" s="79"/>
+    </row>
+    <row r="91" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="27" t="str">
         <f>'MASTER KEY'!A91</f>
         <v>var00094</v>
@@ -11167,8 +11273,9 @@
       <c r="F91" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G91" s="79"/>
+    </row>
+    <row r="92" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="27" t="str">
         <f>'MASTER KEY'!A92</f>
         <v>var00095</v>
@@ -11190,8 +11297,9 @@
       <c r="F92" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G92" s="79"/>
+    </row>
+    <row r="93" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="27" t="str">
         <f>'MASTER KEY'!A93</f>
         <v>var00096</v>
@@ -11213,8 +11321,9 @@
       <c r="F93" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G93" s="79"/>
+    </row>
+    <row r="94" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="27" t="str">
         <f>'MASTER KEY'!A94</f>
         <v>var00097</v>
@@ -11236,8 +11345,9 @@
       <c r="F94" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G94" s="79"/>
+    </row>
+    <row r="95" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="27" t="str">
         <f>'MASTER KEY'!A95</f>
         <v>var00098</v>
@@ -11259,8 +11369,9 @@
       <c r="F95" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G95" s="79"/>
+    </row>
+    <row r="96" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="27" t="str">
         <f>'MASTER KEY'!A96</f>
         <v>var00099</v>
@@ -11282,8 +11393,9 @@
       <c r="F96" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G96" s="79"/>
+    </row>
+    <row r="97" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="27" t="str">
         <f>'MASTER KEY'!A97</f>
         <v>var00100</v>
@@ -11305,8 +11417,9 @@
       <c r="F97" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G97" s="79"/>
+    </row>
+    <row r="98" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="27" t="str">
         <f>'MASTER KEY'!A98</f>
         <v>var00101</v>
@@ -11328,8 +11441,9 @@
       <c r="F98" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G98" s="79"/>
+    </row>
+    <row r="99" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="27" t="str">
         <f>'MASTER KEY'!A99</f>
         <v>var00103</v>
@@ -11351,8 +11465,9 @@
       <c r="F99" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G99" s="79"/>
+    </row>
+    <row r="100" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="27" t="str">
         <f>'MASTER KEY'!A100</f>
         <v>var00104</v>
@@ -11374,8 +11489,9 @@
       <c r="F100" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G100" s="79"/>
+    </row>
+    <row r="101" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="27" t="str">
         <f>'MASTER KEY'!A101</f>
         <v>var00105</v>
@@ -11397,8 +11513,9 @@
       <c r="F101" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G101" s="79"/>
+    </row>
+    <row r="102" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="27" t="str">
         <f>'MASTER KEY'!A102</f>
         <v>var00106</v>
@@ -11420,8 +11537,9 @@
       <c r="F102" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G102" s="79"/>
+    </row>
+    <row r="103" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="27" t="str">
         <f>'MASTER KEY'!A103</f>
         <v>var00107</v>
@@ -11443,8 +11561,9 @@
       <c r="F103" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G103" s="79"/>
+    </row>
+    <row r="104" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="27" t="str">
         <f>'MASTER KEY'!A104</f>
         <v>var00108</v>
@@ -11466,8 +11585,9 @@
       <c r="F104" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G104" s="79"/>
+    </row>
+    <row r="105" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="27" t="str">
         <f>'MASTER KEY'!A105</f>
         <v>var00109</v>
@@ -11489,8 +11609,9 @@
       <c r="F105" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G105" s="79"/>
+    </row>
+    <row r="106" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="27" t="str">
         <f>'MASTER KEY'!A106</f>
         <v>var00110</v>
@@ -11512,8 +11633,9 @@
       <c r="F106" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G106" s="79"/>
+    </row>
+    <row r="107" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="27" t="str">
         <f>'MASTER KEY'!A107</f>
         <v>var00111</v>
@@ -11535,8 +11657,9 @@
       <c r="F107" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G107" s="79"/>
+    </row>
+    <row r="108" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="27" t="str">
         <f>'MASTER KEY'!A108</f>
         <v>var00112</v>
@@ -11558,8 +11681,9 @@
       <c r="F108" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G108" s="79"/>
+    </row>
+    <row r="109" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="27" t="str">
         <f>'MASTER KEY'!A109</f>
         <v>var00113</v>
@@ -11581,8 +11705,9 @@
       <c r="F109" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G109" s="79"/>
+    </row>
+    <row r="110" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="27" t="str">
         <f>'MASTER KEY'!A110</f>
         <v>var00114</v>
@@ -11604,8 +11729,9 @@
       <c r="F110" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G110" s="79"/>
+    </row>
+    <row r="111" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="27" t="str">
         <f>'MASTER KEY'!A111</f>
         <v>var00115</v>
@@ -11627,8 +11753,9 @@
       <c r="F111" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G111" s="79"/>
+    </row>
+    <row r="112" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="27" t="str">
         <f>'MASTER KEY'!A112</f>
         <v>var00116</v>
@@ -11650,8 +11777,9 @@
       <c r="F112" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G112" s="79"/>
+    </row>
+    <row r="113" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="27" t="str">
         <f>'MASTER KEY'!A113</f>
         <v>var00117</v>
@@ -11673,8 +11801,9 @@
       <c r="F113" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G113" s="79"/>
+    </row>
+    <row r="114" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="27" t="str">
         <f>'MASTER KEY'!A114</f>
         <v>var00118</v>
@@ -11696,8 +11825,9 @@
       <c r="F114" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G114" s="79"/>
+    </row>
+    <row r="115" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="27" t="str">
         <f>'MASTER KEY'!A115</f>
         <v>var00119</v>
@@ -11719,8 +11849,9 @@
       <c r="F115" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G115" s="79"/>
+    </row>
+    <row r="116" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="27" t="str">
         <f>'MASTER KEY'!A116</f>
         <v>var00120</v>
@@ -11742,8 +11873,9 @@
       <c r="F116" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G116" s="79"/>
+    </row>
+    <row r="117" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="27" t="str">
         <f>'MASTER KEY'!A117</f>
         <v>var00121</v>
@@ -11765,8 +11897,9 @@
       <c r="F117" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G117" s="79"/>
+    </row>
+    <row r="118" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="27" t="str">
         <f>'MASTER KEY'!A118</f>
         <v>var00122</v>
@@ -11788,8 +11921,9 @@
       <c r="F118" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G118" s="79"/>
+    </row>
+    <row r="119" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="27" t="str">
         <f>'MASTER KEY'!A119</f>
         <v>var00123</v>
@@ -11811,8 +11945,9 @@
       <c r="F119" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G119" s="79"/>
+    </row>
+    <row r="120" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="27" t="str">
         <f>'MASTER KEY'!A120</f>
         <v>var00124</v>
@@ -11834,8 +11969,9 @@
       <c r="F120" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G120" s="79"/>
+    </row>
+    <row r="121" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="27" t="str">
         <f>'MASTER KEY'!A121</f>
         <v>var00125</v>
@@ -11857,8 +11993,9 @@
       <c r="F121" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G121" s="79"/>
+    </row>
+    <row r="122" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="27" t="str">
         <f>'MASTER KEY'!A122</f>
         <v>var00126</v>
@@ -11880,8 +12017,9 @@
       <c r="F122" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G122" s="79"/>
+    </row>
+    <row r="123" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="27" t="str">
         <f>'MASTER KEY'!A123</f>
         <v>var00127</v>
@@ -11903,8 +12041,9 @@
       <c r="F123" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G123" s="79"/>
+    </row>
+    <row r="124" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="27" t="str">
         <f>'MASTER KEY'!A124</f>
         <v>var00128</v>
@@ -11926,8 +12065,9 @@
       <c r="F124" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G124" s="79"/>
+    </row>
+    <row r="125" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="27" t="str">
         <f>'MASTER KEY'!A125</f>
         <v>var00129</v>
@@ -11950,7 +12090,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="27" t="str">
         <f>'MASTER KEY'!A126</f>
         <v>var00130</v>
@@ -11973,7 +12113,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="27" t="str">
         <f>'MASTER KEY'!A127</f>
         <v>var00131</v>
@@ -11996,7 +12136,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="27" t="str">
         <f>'MASTER KEY'!A128</f>
         <v>var00132</v>
@@ -13117,7 +13257,7 @@
         <v>µmol/m2/s</v>
       </c>
       <c r="D176" s="11" t="s">
-        <v>1163</v>
+        <v>2523</v>
       </c>
       <c r="E176" s="27" t="s">
         <v>1152</v>

</xml_diff>

<commit_message>
individual phytoplankton species marvl plot and organisation
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/updates/tassielakes-data/data-governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFA11DE-FBE4-C447-956D-18B73C73CC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D5D973-B2D4-D942-B88B-291B8C9DDA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6637" uniqueCount="2524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7206" uniqueCount="2639">
   <si>
     <t>//</t>
   </si>
@@ -8132,6 +8132,351 @@
   </si>
   <si>
     <t>WQ_DIAG_TOT_PAR_OLD</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_ACHNANTHES</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_ASTERIONELLA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_AULACOSEIRA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_CYCLOTELLA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_CYMBELLA_HAUCKII</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_DIATOMA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_FRAGILARIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_GOMPHONEMA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_NAVICULA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_NITZSCHIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_SYNEDRA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_ULNARIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_UROSOLENIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DIATOM_UNID_DIATOM_BACILLARIALE</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHARA_COSMOCLADIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHARA_ELAKATOTHRIX</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHARA_EUASTRUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHARA_EUDORINA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHARA_MESOTAENIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHARA_ONYCHONEMA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHARA_SPONDYLOSIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHARA_TEILINGIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHARA_ZYGNEMA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN__ANKISTRODESMUS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN__ANKYRA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_BOTRYCOCCUS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_CHLAMYDOMONAS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_CHLOROGONIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_CHODATELLA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_CLOSTERIOPSIS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_CLOSTERIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_COELASTRUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_COMASIELLA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_COSMARIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_CRUCIGENIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_CRUCIGENIELLA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_DESMODESMUS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_DICTYOSPHAERIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_GLOEOCYSTIS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_GOLENKINIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_GOLENKINIOPSIS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_GONIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_KIRCHNERIELLA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_LAGERHEIMIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_MICRACTINIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_MICROSPORA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_MONORAPHIDIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_MOUGEOTIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_NEPHROCYTIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_OOCYSTIS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_PANDORINA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_PAULSCHULZIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_PEDIASTRUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_PLANKTOSPHAERIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_PYRAMIMONAS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_QUADRIGULA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_SCENEDESMUS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_SPHAERELLOPSIS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_SPHAEROCYSTIS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_SPHAEROZOSMA_VERTEBRATUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_STAURASTRUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_STAURODESMUS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_TETRAEDRON</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_ULOTHRIX</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_VOLVOX</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHRYSO_DINOBRYON</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHRYSO_GLOBULIFERA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHRYSO_MALLOMONAS_AKROKOMOS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHRYSO_MALLOMONAS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CHRYSO_SYNURA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CRYPTO_CHROOMONAS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CRYPTO_CRYPTOMONAS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CRYPTO_UNIDENTIFIED_CRYPTOMONAD</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_ANABAENA_BERGII</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_ANABAENA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_ANABAENOPSIS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_ANATHECE</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_APHANOCAPSA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_APHNOTHECE1</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_APHNOTHECE</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_BORZIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_CHROOCOCCUS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_CYANODICTYON</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_DOLICHOSPERMUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_GEITLERINEMA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_GLOEOCAPSA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_GLOEOTHECE</t>
+  </si>
+  <si>
+    <t>Cyanobacteria (Merismopedia sp.)</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_MERISMOPEDIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_MICROCYSTIS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_MYXOBAKTRON</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_NOID_CYANOPHYTE</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_NODULARIA_SPUMIGENA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_PHORMIDIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_PSEUDANABAENA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_RHABDODERMA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_RHABDOGLOEA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_SNOWELLA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_BGA_SYNECHOCOCCUS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DINO_GYMNODINIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_DINO_PERIDINIUM</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_EUGLE_EUGLENA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_EUGLE_PHACUS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_EUGLE_TRACHELOMONAS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_OCHRO_APEDINELLA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_OCHRO_CHRYSOCOCCUS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_OCHRO_CHRYSOSPHAERELLA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_OCHRO_EPITHEMIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_OCHRO_KEPHYRION</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_OCHRO_NAEGELIELLA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_OCHRO_OCHROMONAS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_OCHRO_RHOPALODIA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_OCHRO_SPINIFEROMONAS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_OCHRO_SURIRELLA</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_OCHRO_UROGLENA</t>
   </si>
 </sst>
 </file>
@@ -9060,20 +9405,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G338"/>
+  <dimension ref="A1:G451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="F257" sqref="F257"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A447" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D462" sqref="D462"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16745,9 +17091,2284 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A338" s="6" t="s">
+        <v>2141</v>
+      </c>
       <c r="B338" s="6" t="s">
-        <v>415</v>
+        <v>2142</v>
+      </c>
+      <c r="C338" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D338" s="24" t="s">
+        <v>2524</v>
+      </c>
+      <c r="E338" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F338" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A339" s="6" t="s">
+        <v>2143</v>
+      </c>
+      <c r="B339" t="s">
+        <v>2144</v>
+      </c>
+      <c r="C339" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D339" s="24" t="s">
+        <v>2525</v>
+      </c>
+      <c r="E339" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F339" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A340" s="6" t="s">
+        <v>2145</v>
+      </c>
+      <c r="B340" t="s">
+        <v>2146</v>
+      </c>
+      <c r="C340" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D340" s="24" t="s">
+        <v>2526</v>
+      </c>
+      <c r="E340" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F340" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A341" s="6" t="s">
+        <v>2147</v>
+      </c>
+      <c r="B341" t="s">
+        <v>2148</v>
+      </c>
+      <c r="C341" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D341" s="24" t="s">
+        <v>2527</v>
+      </c>
+      <c r="E341" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F341" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A342" s="6" t="s">
+        <v>2149</v>
+      </c>
+      <c r="B342" t="s">
+        <v>2150</v>
+      </c>
+      <c r="C342" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D342" s="24" t="s">
+        <v>2528</v>
+      </c>
+      <c r="E342" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F342" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A343" s="6" t="s">
+        <v>2151</v>
+      </c>
+      <c r="B343" t="s">
+        <v>2152</v>
+      </c>
+      <c r="C343" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D343" s="24" t="s">
+        <v>2529</v>
+      </c>
+      <c r="E343" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F343" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A344" s="6" t="s">
+        <v>2153</v>
+      </c>
+      <c r="B344" t="s">
+        <v>2154</v>
+      </c>
+      <c r="C344" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D344" s="24" t="s">
+        <v>2530</v>
+      </c>
+      <c r="E344" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F344" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A345" s="6" t="s">
+        <v>2155</v>
+      </c>
+      <c r="B345" t="s">
+        <v>2156</v>
+      </c>
+      <c r="C345" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D345" s="24" t="s">
+        <v>2531</v>
+      </c>
+      <c r="E345" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F345" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A346" s="6" t="s">
+        <v>2157</v>
+      </c>
+      <c r="B346" t="s">
+        <v>2158</v>
+      </c>
+      <c r="C346" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D346" s="24" t="s">
+        <v>2532</v>
+      </c>
+      <c r="E346" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F346" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A347" s="6" t="s">
+        <v>2159</v>
+      </c>
+      <c r="B347" t="s">
+        <v>2160</v>
+      </c>
+      <c r="C347" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D347" s="24" t="s">
+        <v>2533</v>
+      </c>
+      <c r="E347" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F347" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A348" s="6" t="s">
+        <v>2161</v>
+      </c>
+      <c r="B348" t="s">
+        <v>2162</v>
+      </c>
+      <c r="C348" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D348" s="24" t="s">
+        <v>2534</v>
+      </c>
+      <c r="E348" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F348" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A349" s="6" t="s">
+        <v>2163</v>
+      </c>
+      <c r="B349" t="s">
+        <v>2164</v>
+      </c>
+      <c r="C349" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D349" s="24" t="s">
+        <v>2535</v>
+      </c>
+      <c r="E349" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F349" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A350" s="6" t="s">
+        <v>2165</v>
+      </c>
+      <c r="B350" t="s">
+        <v>2166</v>
+      </c>
+      <c r="C350" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D350" s="24" t="s">
+        <v>2536</v>
+      </c>
+      <c r="E350" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F350" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A351" s="6" t="s">
+        <v>2167</v>
+      </c>
+      <c r="B351" t="s">
+        <v>2168</v>
+      </c>
+      <c r="C351" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D351" s="24" t="s">
+        <v>2537</v>
+      </c>
+      <c r="E351" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F351" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A352" s="6" t="s">
+        <v>2175</v>
+      </c>
+      <c r="B352" t="s">
+        <v>2176</v>
+      </c>
+      <c r="C352" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D352" s="24" t="s">
+        <v>2538</v>
+      </c>
+      <c r="E352" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F352" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A353" s="6" t="s">
+        <v>2177</v>
+      </c>
+      <c r="B353" t="s">
+        <v>2178</v>
+      </c>
+      <c r="C353" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D353" s="24" t="s">
+        <v>2539</v>
+      </c>
+      <c r="E353" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F353" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A354" s="6" t="s">
+        <v>2179</v>
+      </c>
+      <c r="B354" t="s">
+        <v>2180</v>
+      </c>
+      <c r="C354" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D354" s="24" t="s">
+        <v>2540</v>
+      </c>
+      <c r="E354" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F354" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A355" s="6" t="s">
+        <v>2181</v>
+      </c>
+      <c r="B355" t="s">
+        <v>2182</v>
+      </c>
+      <c r="C355" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D355" s="24" t="s">
+        <v>2541</v>
+      </c>
+      <c r="E355" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F355" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A356" s="6" t="s">
+        <v>2183</v>
+      </c>
+      <c r="B356" t="s">
+        <v>2184</v>
+      </c>
+      <c r="C356" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D356" s="24" t="s">
+        <v>2542</v>
+      </c>
+      <c r="E356" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F356" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A357" s="6" t="s">
+        <v>2185</v>
+      </c>
+      <c r="B357" t="s">
+        <v>2186</v>
+      </c>
+      <c r="C357" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D357" s="24" t="s">
+        <v>2543</v>
+      </c>
+      <c r="E357" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F357" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A358" s="6" t="s">
+        <v>2187</v>
+      </c>
+      <c r="B358" t="s">
+        <v>2188</v>
+      </c>
+      <c r="C358" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D358" s="24" t="s">
+        <v>2544</v>
+      </c>
+      <c r="E358" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F358" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A359" s="6" t="s">
+        <v>2189</v>
+      </c>
+      <c r="B359" t="s">
+        <v>2190</v>
+      </c>
+      <c r="C359" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D359" s="24" t="s">
+        <v>2545</v>
+      </c>
+      <c r="E359" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F359" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A360" s="6" t="s">
+        <v>2191</v>
+      </c>
+      <c r="B360" t="s">
+        <v>2192</v>
+      </c>
+      <c r="C360" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D360" s="24" t="s">
+        <v>2546</v>
+      </c>
+      <c r="E360" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F360" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A361" s="6" t="s">
+        <v>2195</v>
+      </c>
+      <c r="B361" t="s">
+        <v>2196</v>
+      </c>
+      <c r="C361" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D361" s="24" t="s">
+        <v>2547</v>
+      </c>
+      <c r="E361" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F361" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A362" s="6" t="s">
+        <v>2197</v>
+      </c>
+      <c r="B362" t="s">
+        <v>2198</v>
+      </c>
+      <c r="C362" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D362" s="24" t="s">
+        <v>2548</v>
+      </c>
+      <c r="E362" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F362" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A363" s="6" t="s">
+        <v>2199</v>
+      </c>
+      <c r="B363" t="s">
+        <v>2200</v>
+      </c>
+      <c r="C363" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D363" s="24" t="s">
+        <v>2549</v>
+      </c>
+      <c r="E363" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F363" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A364" s="6" t="s">
+        <v>2201</v>
+      </c>
+      <c r="B364" t="s">
+        <v>2202</v>
+      </c>
+      <c r="C364" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D364" s="24" t="s">
+        <v>2550</v>
+      </c>
+      <c r="E364" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F364" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A365" s="6" t="s">
+        <v>2203</v>
+      </c>
+      <c r="B365" t="s">
+        <v>2204</v>
+      </c>
+      <c r="C365" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D365" s="24" t="s">
+        <v>2551</v>
+      </c>
+      <c r="E365" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F365" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A366" s="6" t="s">
+        <v>2205</v>
+      </c>
+      <c r="B366" t="s">
+        <v>2206</v>
+      </c>
+      <c r="C366" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D366" s="24" t="s">
+        <v>2552</v>
+      </c>
+      <c r="E366" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F366" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A367" s="6" t="s">
+        <v>2207</v>
+      </c>
+      <c r="B367" t="s">
+        <v>2208</v>
+      </c>
+      <c r="C367" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D367" s="24" t="s">
+        <v>2553</v>
+      </c>
+      <c r="E367" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F367" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A368" s="6" t="s">
+        <v>2209</v>
+      </c>
+      <c r="B368" t="s">
+        <v>2210</v>
+      </c>
+      <c r="C368" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D368" s="24" t="s">
+        <v>2554</v>
+      </c>
+      <c r="E368" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F368" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A369" s="6" t="s">
+        <v>2211</v>
+      </c>
+      <c r="B369" t="s">
+        <v>2212</v>
+      </c>
+      <c r="C369" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D369" s="24" t="s">
+        <v>2555</v>
+      </c>
+      <c r="E369" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F369" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A370" s="6" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B370" t="s">
+        <v>2214</v>
+      </c>
+      <c r="C370" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D370" s="24" t="s">
+        <v>2556</v>
+      </c>
+      <c r="E370" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F370" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A371" s="6" t="s">
+        <v>2215</v>
+      </c>
+      <c r="B371" t="s">
+        <v>2216</v>
+      </c>
+      <c r="C371" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D371" s="24" t="s">
+        <v>2557</v>
+      </c>
+      <c r="E371" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F371" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A372" s="6" t="s">
+        <v>2217</v>
+      </c>
+      <c r="B372" t="s">
+        <v>2218</v>
+      </c>
+      <c r="C372" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D372" s="24" t="s">
+        <v>2558</v>
+      </c>
+      <c r="E372" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F372" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A373" s="6" t="s">
+        <v>2219</v>
+      </c>
+      <c r="B373" t="s">
+        <v>2220</v>
+      </c>
+      <c r="C373" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D373" s="24" t="s">
+        <v>2559</v>
+      </c>
+      <c r="E373" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F373" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A374" s="6" t="s">
+        <v>2221</v>
+      </c>
+      <c r="B374" t="s">
+        <v>2222</v>
+      </c>
+      <c r="C374" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D374" s="24" t="s">
+        <v>2560</v>
+      </c>
+      <c r="E374" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F374" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A375" s="6" t="s">
+        <v>2223</v>
+      </c>
+      <c r="B375" t="s">
+        <v>2224</v>
+      </c>
+      <c r="C375" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D375" s="24" t="s">
+        <v>2561</v>
+      </c>
+      <c r="E375" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F375" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A376" s="6" t="s">
+        <v>2225</v>
+      </c>
+      <c r="B376" t="s">
+        <v>2226</v>
+      </c>
+      <c r="C376" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D376" s="24" t="s">
+        <v>2562</v>
+      </c>
+      <c r="E376" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F376" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A377" s="6" t="s">
+        <v>2227</v>
+      </c>
+      <c r="B377" t="s">
+        <v>2228</v>
+      </c>
+      <c r="C377" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D377" s="24" t="s">
+        <v>2563</v>
+      </c>
+      <c r="E377" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F377" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A378" s="6" t="s">
+        <v>2229</v>
+      </c>
+      <c r="B378" t="s">
+        <v>2230</v>
+      </c>
+      <c r="C378" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D378" s="24" t="s">
+        <v>2564</v>
+      </c>
+      <c r="E378" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F378" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A379" s="6" t="s">
+        <v>2231</v>
+      </c>
+      <c r="B379" t="s">
+        <v>2232</v>
+      </c>
+      <c r="C379" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D379" s="24" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E379" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F379" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A380" s="6" t="s">
+        <v>2233</v>
+      </c>
+      <c r="B380" t="s">
+        <v>2234</v>
+      </c>
+      <c r="C380" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D380" s="24" t="s">
+        <v>2566</v>
+      </c>
+      <c r="E380" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F380" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A381" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="B381" t="s">
+        <v>2236</v>
+      </c>
+      <c r="C381" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D381" s="24" t="s">
+        <v>2567</v>
+      </c>
+      <c r="E381" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F381" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A382" s="6" t="s">
+        <v>2237</v>
+      </c>
+      <c r="B382" t="s">
+        <v>2238</v>
+      </c>
+      <c r="C382" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D382" s="24" t="s">
+        <v>2568</v>
+      </c>
+      <c r="E382" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F382" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A383" s="6" t="s">
+        <v>2239</v>
+      </c>
+      <c r="B383" t="s">
+        <v>2240</v>
+      </c>
+      <c r="C383" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D383" s="24" t="s">
+        <v>2569</v>
+      </c>
+      <c r="E383" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F383" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A384" s="6" t="s">
+        <v>2241</v>
+      </c>
+      <c r="B384" t="s">
+        <v>2242</v>
+      </c>
+      <c r="C384" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D384" s="24" t="s">
+        <v>2570</v>
+      </c>
+      <c r="E384" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F384" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A385" s="6" t="s">
+        <v>2243</v>
+      </c>
+      <c r="B385" t="s">
+        <v>2244</v>
+      </c>
+      <c r="C385" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D385" s="24" t="s">
+        <v>2571</v>
+      </c>
+      <c r="E385" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F385" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A386" s="6" t="s">
+        <v>2245</v>
+      </c>
+      <c r="B386" t="s">
+        <v>2246</v>
+      </c>
+      <c r="C386" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D386" s="24" t="s">
+        <v>2572</v>
+      </c>
+      <c r="E386" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F386" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A387" s="6" t="s">
+        <v>2247</v>
+      </c>
+      <c r="B387" t="s">
+        <v>2248</v>
+      </c>
+      <c r="C387" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D387" s="24" t="s">
+        <v>2573</v>
+      </c>
+      <c r="E387" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F387" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A388" s="6" t="s">
+        <v>2249</v>
+      </c>
+      <c r="B388" t="s">
+        <v>2250</v>
+      </c>
+      <c r="C388" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D388" s="24" t="s">
+        <v>2574</v>
+      </c>
+      <c r="E388" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F388" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A389" s="6" t="s">
+        <v>2251</v>
+      </c>
+      <c r="B389" t="s">
+        <v>2252</v>
+      </c>
+      <c r="C389" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D389" s="24" t="s">
+        <v>2575</v>
+      </c>
+      <c r="E389" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F389" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A390" s="6" t="s">
+        <v>2253</v>
+      </c>
+      <c r="B390" t="s">
+        <v>2254</v>
+      </c>
+      <c r="C390" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D390" s="24" t="s">
+        <v>2576</v>
+      </c>
+      <c r="E390" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F390" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A391" s="6" t="s">
+        <v>2255</v>
+      </c>
+      <c r="B391" t="s">
+        <v>2256</v>
+      </c>
+      <c r="C391" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D391" s="24" t="s">
+        <v>2577</v>
+      </c>
+      <c r="E391" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F391" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A392" s="6" t="s">
+        <v>2257</v>
+      </c>
+      <c r="B392" t="s">
+        <v>2258</v>
+      </c>
+      <c r="C392" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D392" s="24" t="s">
+        <v>2578</v>
+      </c>
+      <c r="E392" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F392" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A393" s="6" t="s">
+        <v>2259</v>
+      </c>
+      <c r="B393" t="s">
+        <v>2260</v>
+      </c>
+      <c r="C393" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D393" s="24" t="s">
+        <v>2579</v>
+      </c>
+      <c r="E393" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F393" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A394" s="6" t="s">
+        <v>2261</v>
+      </c>
+      <c r="B394" t="s">
+        <v>2262</v>
+      </c>
+      <c r="C394" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D394" s="24" t="s">
+        <v>2580</v>
+      </c>
+      <c r="E394" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F394" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A395" s="6" t="s">
+        <v>2263</v>
+      </c>
+      <c r="B395" t="s">
+        <v>2264</v>
+      </c>
+      <c r="C395" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D395" s="24" t="s">
+        <v>2581</v>
+      </c>
+      <c r="E395" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F395" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A396" s="6" t="s">
+        <v>2265</v>
+      </c>
+      <c r="B396" t="s">
+        <v>2266</v>
+      </c>
+      <c r="C396" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D396" s="24" t="s">
+        <v>2582</v>
+      </c>
+      <c r="E396" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F396" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A397" s="6" t="s">
+        <v>2267</v>
+      </c>
+      <c r="B397" t="s">
+        <v>2268</v>
+      </c>
+      <c r="C397" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D397" s="24" t="s">
+        <v>2583</v>
+      </c>
+      <c r="E397" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F397" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A398" s="6" t="s">
+        <v>2269</v>
+      </c>
+      <c r="B398" t="s">
+        <v>2270</v>
+      </c>
+      <c r="C398" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D398" s="24" t="s">
+        <v>2584</v>
+      </c>
+      <c r="E398" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F398" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A399" s="6" t="s">
+        <v>2271</v>
+      </c>
+      <c r="B399" t="s">
+        <v>2272</v>
+      </c>
+      <c r="C399" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D399" s="24" t="s">
+        <v>2585</v>
+      </c>
+      <c r="E399" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F399" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A400" s="6" t="s">
+        <v>2273</v>
+      </c>
+      <c r="B400" t="s">
+        <v>2274</v>
+      </c>
+      <c r="C400" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D400" s="24" t="s">
+        <v>2586</v>
+      </c>
+      <c r="E400" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F400" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A401" s="6" t="s">
+        <v>2275</v>
+      </c>
+      <c r="B401" t="s">
+        <v>2276</v>
+      </c>
+      <c r="C401" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D401" s="24" t="s">
+        <v>2587</v>
+      </c>
+      <c r="E401" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F401" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A402" s="6" t="s">
+        <v>2277</v>
+      </c>
+      <c r="B402" t="s">
+        <v>2278</v>
+      </c>
+      <c r="C402" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D402" s="24" t="s">
+        <v>2588</v>
+      </c>
+      <c r="E402" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F402" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A403" s="6" t="s">
+        <v>2283</v>
+      </c>
+      <c r="B403" t="s">
+        <v>2284</v>
+      </c>
+      <c r="C403" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D403" s="24" t="s">
+        <v>2589</v>
+      </c>
+      <c r="E403" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F403" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A404" s="6" t="s">
+        <v>2285</v>
+      </c>
+      <c r="B404" t="s">
+        <v>2286</v>
+      </c>
+      <c r="C404" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D404" s="24" t="s">
+        <v>2590</v>
+      </c>
+      <c r="E404" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F404" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A405" s="6" t="s">
+        <v>2287</v>
+      </c>
+      <c r="B405" t="s">
+        <v>2288</v>
+      </c>
+      <c r="C405" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D405" s="24" t="s">
+        <v>2591</v>
+      </c>
+      <c r="E405" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F405" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A406" s="6" t="s">
+        <v>2289</v>
+      </c>
+      <c r="B406" t="s">
+        <v>2290</v>
+      </c>
+      <c r="C406" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D406" s="24" t="s">
+        <v>2592</v>
+      </c>
+      <c r="E406" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F406" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="407" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A407" s="6" t="s">
+        <v>2291</v>
+      </c>
+      <c r="B407" t="s">
+        <v>2292</v>
+      </c>
+      <c r="C407" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D407" s="24" t="s">
+        <v>2593</v>
+      </c>
+      <c r="E407" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F407" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A408" s="6" t="s">
+        <v>2295</v>
+      </c>
+      <c r="B408" t="s">
+        <v>2296</v>
+      </c>
+      <c r="C408" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D408" s="24" t="s">
+        <v>2594</v>
+      </c>
+      <c r="E408" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F408" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="409" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A409" s="6" t="s">
+        <v>2297</v>
+      </c>
+      <c r="B409" t="s">
+        <v>2298</v>
+      </c>
+      <c r="C409" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D409" s="24" t="s">
+        <v>2595</v>
+      </c>
+      <c r="E409" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F409" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="410" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A410" s="6" t="s">
+        <v>2299</v>
+      </c>
+      <c r="B410" t="s">
+        <v>2300</v>
+      </c>
+      <c r="C410" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D410" s="24" t="s">
+        <v>2596</v>
+      </c>
+      <c r="E410" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F410" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="411" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A411" s="6" t="s">
+        <v>2301</v>
+      </c>
+      <c r="B411" t="s">
+        <v>2302</v>
+      </c>
+      <c r="C411" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D411" s="24" t="s">
+        <v>2597</v>
+      </c>
+      <c r="E411" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F411" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="412" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A412" s="6" t="s">
+        <v>2303</v>
+      </c>
+      <c r="B412" t="s">
+        <v>2304</v>
+      </c>
+      <c r="C412" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D412" s="24" t="s">
+        <v>2598</v>
+      </c>
+      <c r="E412" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F412" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="413" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A413" s="6" t="s">
+        <v>2305</v>
+      </c>
+      <c r="B413" t="s">
+        <v>2306</v>
+      </c>
+      <c r="C413" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D413" s="24" t="s">
+        <v>2599</v>
+      </c>
+      <c r="E413" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F413" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="414" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A414" s="6" t="s">
+        <v>2307</v>
+      </c>
+      <c r="B414" t="s">
+        <v>2308</v>
+      </c>
+      <c r="C414" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D414" s="24" t="s">
+        <v>2600</v>
+      </c>
+      <c r="E414" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F414" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="415" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A415" s="6" t="s">
+        <v>2309</v>
+      </c>
+      <c r="B415" t="s">
+        <v>2310</v>
+      </c>
+      <c r="C415" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D415" s="24" t="s">
+        <v>2601</v>
+      </c>
+      <c r="E415" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F415" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A416" s="6" t="s">
+        <v>2311</v>
+      </c>
+      <c r="B416" t="s">
+        <v>2312</v>
+      </c>
+      <c r="C416" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D416" s="24" t="s">
+        <v>2602</v>
+      </c>
+      <c r="E416" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F416" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A417" s="6" t="s">
+        <v>2313</v>
+      </c>
+      <c r="B417" t="s">
+        <v>2314</v>
+      </c>
+      <c r="C417" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D417" s="24" t="s">
+        <v>2603</v>
+      </c>
+      <c r="E417" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F417" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A418" s="6" t="s">
+        <v>2315</v>
+      </c>
+      <c r="B418" t="s">
+        <v>2316</v>
+      </c>
+      <c r="C418" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D418" s="24" t="s">
+        <v>2604</v>
+      </c>
+      <c r="E418" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F418" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="419" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A419" s="6" t="s">
+        <v>2317</v>
+      </c>
+      <c r="B419" t="s">
+        <v>2318</v>
+      </c>
+      <c r="C419" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D419" s="24" t="s">
+        <v>2605</v>
+      </c>
+      <c r="E419" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F419" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A420" s="6" t="s">
+        <v>2319</v>
+      </c>
+      <c r="B420" t="s">
+        <v>2320</v>
+      </c>
+      <c r="C420" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D420" s="24" t="s">
+        <v>2606</v>
+      </c>
+      <c r="E420" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F420" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="421" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A421" s="6" t="s">
+        <v>2321</v>
+      </c>
+      <c r="B421" t="s">
+        <v>2322</v>
+      </c>
+      <c r="C421" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D421" s="24" t="s">
+        <v>2607</v>
+      </c>
+      <c r="E421" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F421" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A422" s="6" t="s">
+        <v>2323</v>
+      </c>
+      <c r="B422" t="s">
+        <v>2324</v>
+      </c>
+      <c r="C422" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D422" s="24" t="s">
+        <v>2608</v>
+      </c>
+      <c r="E422" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F422" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A423" s="6" t="s">
+        <v>2325</v>
+      </c>
+      <c r="B423" t="s">
+        <v>2326</v>
+      </c>
+      <c r="C423" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D423" s="24" t="s">
+        <v>2609</v>
+      </c>
+      <c r="E423" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F423" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A424" s="6" t="s">
+        <v>2327</v>
+      </c>
+      <c r="B424" t="s">
+        <v>2328</v>
+      </c>
+      <c r="C424" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D424" s="24" t="s">
+        <v>2610</v>
+      </c>
+      <c r="E424" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F424" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A425" s="6" t="s">
+        <v>2329</v>
+      </c>
+      <c r="B425" t="s">
+        <v>2611</v>
+      </c>
+      <c r="C425" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D425" s="24" t="s">
+        <v>2612</v>
+      </c>
+      <c r="E425" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F425" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A426" s="6" t="s">
+        <v>2331</v>
+      </c>
+      <c r="B426" t="s">
+        <v>2332</v>
+      </c>
+      <c r="C426" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D426" s="24" t="s">
+        <v>2613</v>
+      </c>
+      <c r="E426" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F426" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A427" s="6" t="s">
+        <v>2333</v>
+      </c>
+      <c r="B427" t="s">
+        <v>2334</v>
+      </c>
+      <c r="C427" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D427" s="24" t="s">
+        <v>2614</v>
+      </c>
+      <c r="E427" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F427" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A428" s="6" t="s">
+        <v>2335</v>
+      </c>
+      <c r="B428" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C428" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D428" s="24" t="s">
+        <v>2615</v>
+      </c>
+      <c r="E428" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F428" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A429" s="6" t="s">
+        <v>2337</v>
+      </c>
+      <c r="B429" t="s">
+        <v>2338</v>
+      </c>
+      <c r="C429" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D429" s="24" t="s">
+        <v>2616</v>
+      </c>
+      <c r="E429" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F429" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A430" s="6" t="s">
+        <v>2339</v>
+      </c>
+      <c r="B430" t="s">
+        <v>2340</v>
+      </c>
+      <c r="C430" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D430" s="24" t="s">
+        <v>2617</v>
+      </c>
+      <c r="E430" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F430" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A431" s="6" t="s">
+        <v>2341</v>
+      </c>
+      <c r="B431" t="s">
+        <v>2342</v>
+      </c>
+      <c r="C431" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D431" s="24" t="s">
+        <v>2618</v>
+      </c>
+      <c r="E431" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F431" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A432" s="6" t="s">
+        <v>2343</v>
+      </c>
+      <c r="B432" t="s">
+        <v>2344</v>
+      </c>
+      <c r="C432" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D432" s="24" t="s">
+        <v>2619</v>
+      </c>
+      <c r="E432" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F432" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A433" s="6" t="s">
+        <v>2345</v>
+      </c>
+      <c r="B433" t="s">
+        <v>2346</v>
+      </c>
+      <c r="C433" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D433" s="24" t="s">
+        <v>2620</v>
+      </c>
+      <c r="E433" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F433" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A434" s="6" t="s">
+        <v>2347</v>
+      </c>
+      <c r="B434" t="s">
+        <v>2348</v>
+      </c>
+      <c r="C434" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D434" s="24" t="s">
+        <v>2621</v>
+      </c>
+      <c r="E434" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F434" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A435" s="6" t="s">
+        <v>2349</v>
+      </c>
+      <c r="B435" t="s">
+        <v>2350</v>
+      </c>
+      <c r="C435" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D435" s="24" t="s">
+        <v>2622</v>
+      </c>
+      <c r="E435" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F435" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A436" s="6" t="s">
+        <v>2353</v>
+      </c>
+      <c r="B436" t="s">
+        <v>2354</v>
+      </c>
+      <c r="C436" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D436" s="24" t="s">
+        <v>2623</v>
+      </c>
+      <c r="E436" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F436" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A437" s="6" t="s">
+        <v>2355</v>
+      </c>
+      <c r="B437" t="s">
+        <v>2356</v>
+      </c>
+      <c r="C437" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D437" s="24" t="s">
+        <v>2624</v>
+      </c>
+      <c r="E437" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F437" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A438" s="6" t="s">
+        <v>2361</v>
+      </c>
+      <c r="B438" t="s">
+        <v>2362</v>
+      </c>
+      <c r="C438" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D438" s="24" t="s">
+        <v>2625</v>
+      </c>
+      <c r="E438" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F438" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A439" s="6" t="s">
+        <v>2363</v>
+      </c>
+      <c r="B439" t="s">
+        <v>2364</v>
+      </c>
+      <c r="C439" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D439" s="24" t="s">
+        <v>2626</v>
+      </c>
+      <c r="E439" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F439" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A440" s="6" t="s">
+        <v>2365</v>
+      </c>
+      <c r="B440" t="s">
+        <v>2366</v>
+      </c>
+      <c r="C440" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D440" s="24" t="s">
+        <v>2627</v>
+      </c>
+      <c r="E440" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F440" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A441" s="6" t="s">
+        <v>2385</v>
+      </c>
+      <c r="B441" t="s">
+        <v>2386</v>
+      </c>
+      <c r="C441" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D441" s="24" t="s">
+        <v>2628</v>
+      </c>
+      <c r="E441" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F441" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A442" s="6" t="s">
+        <v>2387</v>
+      </c>
+      <c r="B442" t="s">
+        <v>2388</v>
+      </c>
+      <c r="C442" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D442" s="24" t="s">
+        <v>2629</v>
+      </c>
+      <c r="E442" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F442" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A443" s="6" t="s">
+        <v>2389</v>
+      </c>
+      <c r="B443" t="s">
+        <v>2390</v>
+      </c>
+      <c r="C443" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D443" s="24" t="s">
+        <v>2630</v>
+      </c>
+      <c r="E443" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F443" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A444" s="6" t="s">
+        <v>2391</v>
+      </c>
+      <c r="B444" t="s">
+        <v>2392</v>
+      </c>
+      <c r="C444" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D444" s="24" t="s">
+        <v>2631</v>
+      </c>
+      <c r="E444" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F444" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A445" s="6" t="s">
+        <v>2393</v>
+      </c>
+      <c r="B445" t="s">
+        <v>2394</v>
+      </c>
+      <c r="C445" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D445" s="24" t="s">
+        <v>2632</v>
+      </c>
+      <c r="E445" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F445" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A446" s="6" t="s">
+        <v>2395</v>
+      </c>
+      <c r="B446" t="s">
+        <v>2396</v>
+      </c>
+      <c r="C446" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D446" s="24" t="s">
+        <v>2633</v>
+      </c>
+      <c r="E446" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F446" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A447" s="6" t="s">
+        <v>2397</v>
+      </c>
+      <c r="B447" t="s">
+        <v>2398</v>
+      </c>
+      <c r="C447" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D447" s="24" t="s">
+        <v>2634</v>
+      </c>
+      <c r="E447" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F447" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A448" s="6" t="s">
+        <v>2399</v>
+      </c>
+      <c r="B448" t="s">
+        <v>2400</v>
+      </c>
+      <c r="C448" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D448" s="24" t="s">
+        <v>2635</v>
+      </c>
+      <c r="E448" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F448" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A449" s="6" t="s">
+        <v>2401</v>
+      </c>
+      <c r="B449" t="s">
+        <v>2402</v>
+      </c>
+      <c r="C449" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D449" s="24" t="s">
+        <v>2636</v>
+      </c>
+      <c r="E449" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F449" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A450" s="6" t="s">
+        <v>2403</v>
+      </c>
+      <c r="B450" t="s">
+        <v>2404</v>
+      </c>
+      <c r="C450" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D450" s="24" t="s">
+        <v>2637</v>
+      </c>
+      <c r="E450" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F450" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A451" s="6" t="s">
+        <v>2405</v>
+      </c>
+      <c r="B451" t="s">
+        <v>2406</v>
+      </c>
+      <c r="C451" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D451" s="24" t="s">
+        <v>2638</v>
+      </c>
+      <c r="E451" s="69" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F451" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -20146,7 +22767,7 @@
   <dimension ref="A1:V555"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A529" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update matfile and marvl plots with woods lake middle surface continuous data
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/updates/tassielakes-data/data-governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541A4881-4285-4148-848B-7D843794DE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013E49CD-CF7B-414D-9270-36B7E4C8A6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7206" uniqueCount="2639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7211" uniqueCount="2640">
   <si>
     <t>//</t>
   </si>
@@ -8477,6 +8477,9 @@
   </si>
   <si>
     <t>Phycocyanin</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_PHYCO</t>
   </si>
 </sst>
 </file>
@@ -9405,11 +9408,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G451"/>
+  <dimension ref="A1:G452"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A447" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D462" sqref="D462"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A424" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D454" sqref="D454"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19368,6 +19371,26 @@
         <v>2459</v>
       </c>
       <c r="F451" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A452" s="6" t="s">
+        <v>2452</v>
+      </c>
+      <c r="B452" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C452" s="24" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D452" s="6" t="s">
+        <v>2639</v>
+      </c>
+      <c r="E452" s="6" t="s">
+        <v>1152</v>
+      </c>
+      <c r="F452" s="5">
         <v>1</v>
       </c>
     </row>
@@ -22766,8 +22789,8 @@
   </sheetPr>
   <dimension ref="A1:V555"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A519" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A522" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K547" sqref="K547"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Processed data and header for BG Algae heterocyte vegetative cell ratio
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/updates/tassielakes-data/data-governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013E49CD-CF7B-414D-9270-36B7E4C8A6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CABF048-A4E2-2447-90D8-C002E47A7496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7211" uniqueCount="2640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7219" uniqueCount="2644">
   <si>
     <t>//</t>
   </si>
@@ -8480,6 +8480,18 @@
   </si>
   <si>
     <t>WQ_DIAG_PHY_PHYCO</t>
+  </si>
+  <si>
+    <t>var00776</t>
+  </si>
+  <si>
+    <t>Heterocyte:Vegetative cell ratio</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_HVR</t>
+  </si>
+  <si>
+    <t>Heterocyte Vegetative cell ratio</t>
   </si>
 </sst>
 </file>
@@ -9408,11 +9420,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G452"/>
+  <dimension ref="A1:G453"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A424" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D454" sqref="D454"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A422" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H432" sqref="H432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19391,6 +19403,26 @@
         <v>1152</v>
       </c>
       <c r="F452" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A453" s="6" t="s">
+        <v>2640</v>
+      </c>
+      <c r="B453" s="6" t="s">
+        <v>2641</v>
+      </c>
+      <c r="C453" s="24" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D453" s="6" t="s">
+        <v>2642</v>
+      </c>
+      <c r="E453" s="6" t="s">
+        <v>1152</v>
+      </c>
+      <c r="F453" s="5">
         <v>1</v>
       </c>
     </row>
@@ -22787,11 +22819,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:V555"/>
+  <dimension ref="A1:V556"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A522" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K547" sqref="K547"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A399" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D406" sqref="D406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35581,6 +35613,17 @@
       </c>
       <c r="K555" s="70" t="s">
         <v>1456</v>
+      </c>
+    </row>
+    <row r="556" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A556" s="6" t="s">
+        <v>2640</v>
+      </c>
+      <c r="B556" s="6" t="s">
+        <v>2643</v>
+      </c>
+      <c r="K556" s="70" t="s">
+        <v>1323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
matfile and marvl plots for BG Algae
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/updates/tassielakes-data/data-governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CABF048-A4E2-2447-90D8-C002E47A7496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0062E13D-8501-F142-9C43-B340ACB2CD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -8200,12 +8200,6 @@
     <t>WQ_DIAG_PHY_CHARA_ZYGNEMA</t>
   </si>
   <si>
-    <t>WQ_DIAG_PHY_GRN__ANKISTRODESMUS</t>
-  </si>
-  <si>
-    <t>WQ_DIAG_PHY_GRN__ANKYRA</t>
-  </si>
-  <si>
     <t>WQ_DIAG_PHY_GRN_BOTRYCOCCUS</t>
   </si>
   <si>
@@ -8492,6 +8486,12 @@
   </si>
   <si>
     <t>Heterocyte Vegetative cell ratio</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_ANKISTRODESMUS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_ANKYRA</t>
   </si>
 </sst>
 </file>
@@ -9422,9 +9422,9 @@
   </sheetPr>
   <dimension ref="A1:G453"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A422" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H432" sqref="H432"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A341" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D362" sqref="D362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17577,7 +17577,7 @@
         <v>2459</v>
       </c>
       <c r="D361" s="24" t="s">
-        <v>2546</v>
+        <v>2642</v>
       </c>
       <c r="E361" s="69" t="s">
         <v>2459</v>
@@ -17597,7 +17597,7 @@
         <v>2459</v>
       </c>
       <c r="D362" s="24" t="s">
-        <v>2547</v>
+        <v>2643</v>
       </c>
       <c r="E362" s="69" t="s">
         <v>2459</v>
@@ -17617,7 +17617,7 @@
         <v>2459</v>
       </c>
       <c r="D363" s="24" t="s">
-        <v>2548</v>
+        <v>2546</v>
       </c>
       <c r="E363" s="69" t="s">
         <v>2459</v>
@@ -17637,7 +17637,7 @@
         <v>2459</v>
       </c>
       <c r="D364" s="24" t="s">
-        <v>2549</v>
+        <v>2547</v>
       </c>
       <c r="E364" s="69" t="s">
         <v>2459</v>
@@ -17657,7 +17657,7 @@
         <v>2459</v>
       </c>
       <c r="D365" s="24" t="s">
-        <v>2550</v>
+        <v>2548</v>
       </c>
       <c r="E365" s="69" t="s">
         <v>2459</v>
@@ -17677,7 +17677,7 @@
         <v>2459</v>
       </c>
       <c r="D366" s="24" t="s">
-        <v>2551</v>
+        <v>2549</v>
       </c>
       <c r="E366" s="69" t="s">
         <v>2459</v>
@@ -17697,7 +17697,7 @@
         <v>2459</v>
       </c>
       <c r="D367" s="24" t="s">
-        <v>2552</v>
+        <v>2550</v>
       </c>
       <c r="E367" s="69" t="s">
         <v>2459</v>
@@ -17717,7 +17717,7 @@
         <v>2459</v>
       </c>
       <c r="D368" s="24" t="s">
-        <v>2553</v>
+        <v>2551</v>
       </c>
       <c r="E368" s="69" t="s">
         <v>2459</v>
@@ -17737,7 +17737,7 @@
         <v>2459</v>
       </c>
       <c r="D369" s="24" t="s">
-        <v>2554</v>
+        <v>2552</v>
       </c>
       <c r="E369" s="69" t="s">
         <v>2459</v>
@@ -17757,7 +17757,7 @@
         <v>2459</v>
       </c>
       <c r="D370" s="24" t="s">
-        <v>2555</v>
+        <v>2553</v>
       </c>
       <c r="E370" s="69" t="s">
         <v>2459</v>
@@ -17777,7 +17777,7 @@
         <v>2459</v>
       </c>
       <c r="D371" s="24" t="s">
-        <v>2556</v>
+        <v>2554</v>
       </c>
       <c r="E371" s="69" t="s">
         <v>2459</v>
@@ -17797,7 +17797,7 @@
         <v>2459</v>
       </c>
       <c r="D372" s="24" t="s">
-        <v>2557</v>
+        <v>2555</v>
       </c>
       <c r="E372" s="69" t="s">
         <v>2459</v>
@@ -17817,7 +17817,7 @@
         <v>2459</v>
       </c>
       <c r="D373" s="24" t="s">
-        <v>2558</v>
+        <v>2556</v>
       </c>
       <c r="E373" s="69" t="s">
         <v>2459</v>
@@ -17837,7 +17837,7 @@
         <v>2459</v>
       </c>
       <c r="D374" s="24" t="s">
-        <v>2559</v>
+        <v>2557</v>
       </c>
       <c r="E374" s="69" t="s">
         <v>2459</v>
@@ -17857,7 +17857,7 @@
         <v>2459</v>
       </c>
       <c r="D375" s="24" t="s">
-        <v>2560</v>
+        <v>2558</v>
       </c>
       <c r="E375" s="69" t="s">
         <v>2459</v>
@@ -17877,7 +17877,7 @@
         <v>2459</v>
       </c>
       <c r="D376" s="24" t="s">
-        <v>2561</v>
+        <v>2559</v>
       </c>
       <c r="E376" s="69" t="s">
         <v>2459</v>
@@ -17897,7 +17897,7 @@
         <v>2459</v>
       </c>
       <c r="D377" s="24" t="s">
-        <v>2562</v>
+        <v>2560</v>
       </c>
       <c r="E377" s="69" t="s">
         <v>2459</v>
@@ -17917,7 +17917,7 @@
         <v>2459</v>
       </c>
       <c r="D378" s="24" t="s">
-        <v>2563</v>
+        <v>2561</v>
       </c>
       <c r="E378" s="69" t="s">
         <v>2459</v>
@@ -17937,7 +17937,7 @@
         <v>2459</v>
       </c>
       <c r="D379" s="24" t="s">
-        <v>2564</v>
+        <v>2562</v>
       </c>
       <c r="E379" s="69" t="s">
         <v>2459</v>
@@ -17957,7 +17957,7 @@
         <v>2459</v>
       </c>
       <c r="D380" s="24" t="s">
-        <v>2565</v>
+        <v>2563</v>
       </c>
       <c r="E380" s="69" t="s">
         <v>2459</v>
@@ -17977,7 +17977,7 @@
         <v>2459</v>
       </c>
       <c r="D381" s="24" t="s">
-        <v>2566</v>
+        <v>2564</v>
       </c>
       <c r="E381" s="69" t="s">
         <v>2459</v>
@@ -17997,7 +17997,7 @@
         <v>2459</v>
       </c>
       <c r="D382" s="24" t="s">
-        <v>2567</v>
+        <v>2565</v>
       </c>
       <c r="E382" s="69" t="s">
         <v>2459</v>
@@ -18017,7 +18017,7 @@
         <v>2459</v>
       </c>
       <c r="D383" s="24" t="s">
-        <v>2568</v>
+        <v>2566</v>
       </c>
       <c r="E383" s="69" t="s">
         <v>2459</v>
@@ -18037,7 +18037,7 @@
         <v>2459</v>
       </c>
       <c r="D384" s="24" t="s">
-        <v>2569</v>
+        <v>2567</v>
       </c>
       <c r="E384" s="69" t="s">
         <v>2459</v>
@@ -18057,7 +18057,7 @@
         <v>2459</v>
       </c>
       <c r="D385" s="24" t="s">
-        <v>2570</v>
+        <v>2568</v>
       </c>
       <c r="E385" s="69" t="s">
         <v>2459</v>
@@ -18077,7 +18077,7 @@
         <v>2459</v>
       </c>
       <c r="D386" s="24" t="s">
-        <v>2571</v>
+        <v>2569</v>
       </c>
       <c r="E386" s="69" t="s">
         <v>2459</v>
@@ -18097,7 +18097,7 @@
         <v>2459</v>
       </c>
       <c r="D387" s="24" t="s">
-        <v>2572</v>
+        <v>2570</v>
       </c>
       <c r="E387" s="69" t="s">
         <v>2459</v>
@@ -18117,7 +18117,7 @@
         <v>2459</v>
       </c>
       <c r="D388" s="24" t="s">
-        <v>2573</v>
+        <v>2571</v>
       </c>
       <c r="E388" s="69" t="s">
         <v>2459</v>
@@ -18137,7 +18137,7 @@
         <v>2459</v>
       </c>
       <c r="D389" s="24" t="s">
-        <v>2574</v>
+        <v>2572</v>
       </c>
       <c r="E389" s="69" t="s">
         <v>2459</v>
@@ -18157,7 +18157,7 @@
         <v>2459</v>
       </c>
       <c r="D390" s="24" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="E390" s="69" t="s">
         <v>2459</v>
@@ -18177,7 +18177,7 @@
         <v>2459</v>
       </c>
       <c r="D391" s="24" t="s">
-        <v>2576</v>
+        <v>2574</v>
       </c>
       <c r="E391" s="69" t="s">
         <v>2459</v>
@@ -18197,7 +18197,7 @@
         <v>2459</v>
       </c>
       <c r="D392" s="24" t="s">
-        <v>2577</v>
+        <v>2575</v>
       </c>
       <c r="E392" s="69" t="s">
         <v>2459</v>
@@ -18217,7 +18217,7 @@
         <v>2459</v>
       </c>
       <c r="D393" s="24" t="s">
-        <v>2578</v>
+        <v>2576</v>
       </c>
       <c r="E393" s="69" t="s">
         <v>2459</v>
@@ -18237,7 +18237,7 @@
         <v>2459</v>
       </c>
       <c r="D394" s="24" t="s">
-        <v>2579</v>
+        <v>2577</v>
       </c>
       <c r="E394" s="69" t="s">
         <v>2459</v>
@@ -18257,7 +18257,7 @@
         <v>2459</v>
       </c>
       <c r="D395" s="24" t="s">
-        <v>2580</v>
+        <v>2578</v>
       </c>
       <c r="E395" s="69" t="s">
         <v>2459</v>
@@ -18277,7 +18277,7 @@
         <v>2459</v>
       </c>
       <c r="D396" s="24" t="s">
-        <v>2581</v>
+        <v>2579</v>
       </c>
       <c r="E396" s="69" t="s">
         <v>2459</v>
@@ -18297,7 +18297,7 @@
         <v>2459</v>
       </c>
       <c r="D397" s="24" t="s">
-        <v>2582</v>
+        <v>2580</v>
       </c>
       <c r="E397" s="69" t="s">
         <v>2459</v>
@@ -18317,7 +18317,7 @@
         <v>2459</v>
       </c>
       <c r="D398" s="24" t="s">
-        <v>2583</v>
+        <v>2581</v>
       </c>
       <c r="E398" s="69" t="s">
         <v>2459</v>
@@ -18337,7 +18337,7 @@
         <v>2459</v>
       </c>
       <c r="D399" s="24" t="s">
-        <v>2584</v>
+        <v>2582</v>
       </c>
       <c r="E399" s="69" t="s">
         <v>2459</v>
@@ -18357,7 +18357,7 @@
         <v>2459</v>
       </c>
       <c r="D400" s="24" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
       <c r="E400" s="69" t="s">
         <v>2459</v>
@@ -18377,7 +18377,7 @@
         <v>2459</v>
       </c>
       <c r="D401" s="24" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
       <c r="E401" s="69" t="s">
         <v>2459</v>
@@ -18397,7 +18397,7 @@
         <v>2459</v>
       </c>
       <c r="D402" s="24" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
       <c r="E402" s="69" t="s">
         <v>2459</v>
@@ -18417,7 +18417,7 @@
         <v>2459</v>
       </c>
       <c r="D403" s="24" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
       <c r="E403" s="69" t="s">
         <v>2459</v>
@@ -18437,7 +18437,7 @@
         <v>2459</v>
       </c>
       <c r="D404" s="24" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
       <c r="E404" s="69" t="s">
         <v>2459</v>
@@ -18457,7 +18457,7 @@
         <v>2459</v>
       </c>
       <c r="D405" s="24" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
       <c r="E405" s="69" t="s">
         <v>2459</v>
@@ -18477,7 +18477,7 @@
         <v>2459</v>
       </c>
       <c r="D406" s="24" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
       <c r="E406" s="69" t="s">
         <v>2459</v>
@@ -18497,7 +18497,7 @@
         <v>2459</v>
       </c>
       <c r="D407" s="24" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
       <c r="E407" s="69" t="s">
         <v>2459</v>
@@ -18517,7 +18517,7 @@
         <v>2459</v>
       </c>
       <c r="D408" s="24" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
       <c r="E408" s="69" t="s">
         <v>2459</v>
@@ -18537,7 +18537,7 @@
         <v>2459</v>
       </c>
       <c r="D409" s="24" t="s">
-        <v>2594</v>
+        <v>2592</v>
       </c>
       <c r="E409" s="69" t="s">
         <v>2459</v>
@@ -18557,7 +18557,7 @@
         <v>2459</v>
       </c>
       <c r="D410" s="24" t="s">
-        <v>2595</v>
+        <v>2593</v>
       </c>
       <c r="E410" s="69" t="s">
         <v>2459</v>
@@ -18577,7 +18577,7 @@
         <v>2459</v>
       </c>
       <c r="D411" s="24" t="s">
-        <v>2596</v>
+        <v>2594</v>
       </c>
       <c r="E411" s="69" t="s">
         <v>2459</v>
@@ -18597,7 +18597,7 @@
         <v>2459</v>
       </c>
       <c r="D412" s="24" t="s">
-        <v>2597</v>
+        <v>2595</v>
       </c>
       <c r="E412" s="69" t="s">
         <v>2459</v>
@@ -18617,7 +18617,7 @@
         <v>2459</v>
       </c>
       <c r="D413" s="24" t="s">
-        <v>2598</v>
+        <v>2596</v>
       </c>
       <c r="E413" s="69" t="s">
         <v>2459</v>
@@ -18637,7 +18637,7 @@
         <v>2459</v>
       </c>
       <c r="D414" s="24" t="s">
-        <v>2599</v>
+        <v>2597</v>
       </c>
       <c r="E414" s="69" t="s">
         <v>2459</v>
@@ -18657,7 +18657,7 @@
         <v>2459</v>
       </c>
       <c r="D415" s="24" t="s">
-        <v>2600</v>
+        <v>2598</v>
       </c>
       <c r="E415" s="69" t="s">
         <v>2459</v>
@@ -18677,7 +18677,7 @@
         <v>2459</v>
       </c>
       <c r="D416" s="24" t="s">
-        <v>2601</v>
+        <v>2599</v>
       </c>
       <c r="E416" s="69" t="s">
         <v>2459</v>
@@ -18697,7 +18697,7 @@
         <v>2459</v>
       </c>
       <c r="D417" s="24" t="s">
-        <v>2602</v>
+        <v>2600</v>
       </c>
       <c r="E417" s="69" t="s">
         <v>2459</v>
@@ -18717,7 +18717,7 @@
         <v>2459</v>
       </c>
       <c r="D418" s="24" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="E418" s="69" t="s">
         <v>2459</v>
@@ -18737,7 +18737,7 @@
         <v>2459</v>
       </c>
       <c r="D419" s="24" t="s">
-        <v>2604</v>
+        <v>2602</v>
       </c>
       <c r="E419" s="69" t="s">
         <v>2459</v>
@@ -18757,7 +18757,7 @@
         <v>2459</v>
       </c>
       <c r="D420" s="24" t="s">
-        <v>2605</v>
+        <v>2603</v>
       </c>
       <c r="E420" s="69" t="s">
         <v>2459</v>
@@ -18777,7 +18777,7 @@
         <v>2459</v>
       </c>
       <c r="D421" s="24" t="s">
-        <v>2606</v>
+        <v>2604</v>
       </c>
       <c r="E421" s="69" t="s">
         <v>2459</v>
@@ -18797,7 +18797,7 @@
         <v>2459</v>
       </c>
       <c r="D422" s="24" t="s">
-        <v>2607</v>
+        <v>2605</v>
       </c>
       <c r="E422" s="69" t="s">
         <v>2459</v>
@@ -18817,7 +18817,7 @@
         <v>2459</v>
       </c>
       <c r="D423" s="24" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
       <c r="E423" s="69" t="s">
         <v>2459</v>
@@ -18837,7 +18837,7 @@
         <v>2459</v>
       </c>
       <c r="D424" s="24" t="s">
-        <v>2609</v>
+        <v>2607</v>
       </c>
       <c r="E424" s="69" t="s">
         <v>2459</v>
@@ -18851,13 +18851,13 @@
         <v>2329</v>
       </c>
       <c r="B425" t="s">
-        <v>2610</v>
+        <v>2608</v>
       </c>
       <c r="C425" s="69" t="s">
         <v>2459</v>
       </c>
       <c r="D425" s="24" t="s">
-        <v>2611</v>
+        <v>2609</v>
       </c>
       <c r="E425" s="69" t="s">
         <v>2459</v>
@@ -18877,7 +18877,7 @@
         <v>2459</v>
       </c>
       <c r="D426" s="24" t="s">
-        <v>2612</v>
+        <v>2610</v>
       </c>
       <c r="E426" s="69" t="s">
         <v>2459</v>
@@ -18897,7 +18897,7 @@
         <v>2459</v>
       </c>
       <c r="D427" s="24" t="s">
-        <v>2613</v>
+        <v>2611</v>
       </c>
       <c r="E427" s="69" t="s">
         <v>2459</v>
@@ -18917,7 +18917,7 @@
         <v>2459</v>
       </c>
       <c r="D428" s="24" t="s">
-        <v>2614</v>
+        <v>2612</v>
       </c>
       <c r="E428" s="69" t="s">
         <v>2459</v>
@@ -18937,7 +18937,7 @@
         <v>2459</v>
       </c>
       <c r="D429" s="24" t="s">
-        <v>2615</v>
+        <v>2613</v>
       </c>
       <c r="E429" s="69" t="s">
         <v>2459</v>
@@ -18957,7 +18957,7 @@
         <v>2459</v>
       </c>
       <c r="D430" s="24" t="s">
-        <v>2616</v>
+        <v>2614</v>
       </c>
       <c r="E430" s="69" t="s">
         <v>2459</v>
@@ -18977,7 +18977,7 @@
         <v>2459</v>
       </c>
       <c r="D431" s="24" t="s">
-        <v>2617</v>
+        <v>2615</v>
       </c>
       <c r="E431" s="69" t="s">
         <v>2459</v>
@@ -18997,7 +18997,7 @@
         <v>2459</v>
       </c>
       <c r="D432" s="24" t="s">
-        <v>2618</v>
+        <v>2616</v>
       </c>
       <c r="E432" s="69" t="s">
         <v>2459</v>
@@ -19017,7 +19017,7 @@
         <v>2459</v>
       </c>
       <c r="D433" s="24" t="s">
-        <v>2619</v>
+        <v>2617</v>
       </c>
       <c r="E433" s="69" t="s">
         <v>2459</v>
@@ -19037,7 +19037,7 @@
         <v>2459</v>
       </c>
       <c r="D434" s="24" t="s">
-        <v>2620</v>
+        <v>2618</v>
       </c>
       <c r="E434" s="69" t="s">
         <v>2459</v>
@@ -19057,7 +19057,7 @@
         <v>2459</v>
       </c>
       <c r="D435" s="24" t="s">
-        <v>2621</v>
+        <v>2619</v>
       </c>
       <c r="E435" s="69" t="s">
         <v>2459</v>
@@ -19077,7 +19077,7 @@
         <v>2459</v>
       </c>
       <c r="D436" s="24" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="E436" s="69" t="s">
         <v>2459</v>
@@ -19097,7 +19097,7 @@
         <v>2459</v>
       </c>
       <c r="D437" s="24" t="s">
-        <v>2623</v>
+        <v>2621</v>
       </c>
       <c r="E437" s="69" t="s">
         <v>2459</v>
@@ -19117,7 +19117,7 @@
         <v>2459</v>
       </c>
       <c r="D438" s="24" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
       <c r="E438" s="69" t="s">
         <v>2459</v>
@@ -19137,7 +19137,7 @@
         <v>2459</v>
       </c>
       <c r="D439" s="24" t="s">
-        <v>2625</v>
+        <v>2623</v>
       </c>
       <c r="E439" s="69" t="s">
         <v>2459</v>
@@ -19157,7 +19157,7 @@
         <v>2459</v>
       </c>
       <c r="D440" s="24" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
       <c r="E440" s="69" t="s">
         <v>2459</v>
@@ -19177,7 +19177,7 @@
         <v>2459</v>
       </c>
       <c r="D441" s="24" t="s">
-        <v>2627</v>
+        <v>2625</v>
       </c>
       <c r="E441" s="69" t="s">
         <v>2459</v>
@@ -19197,7 +19197,7 @@
         <v>2459</v>
       </c>
       <c r="D442" s="24" t="s">
-        <v>2628</v>
+        <v>2626</v>
       </c>
       <c r="E442" s="69" t="s">
         <v>2459</v>
@@ -19217,7 +19217,7 @@
         <v>2459</v>
       </c>
       <c r="D443" s="24" t="s">
-        <v>2629</v>
+        <v>2627</v>
       </c>
       <c r="E443" s="69" t="s">
         <v>2459</v>
@@ -19237,7 +19237,7 @@
         <v>2459</v>
       </c>
       <c r="D444" s="24" t="s">
-        <v>2630</v>
+        <v>2628</v>
       </c>
       <c r="E444" s="69" t="s">
         <v>2459</v>
@@ -19257,7 +19257,7 @@
         <v>2459</v>
       </c>
       <c r="D445" s="24" t="s">
-        <v>2631</v>
+        <v>2629</v>
       </c>
       <c r="E445" s="69" t="s">
         <v>2459</v>
@@ -19277,7 +19277,7 @@
         <v>2459</v>
       </c>
       <c r="D446" s="24" t="s">
-        <v>2632</v>
+        <v>2630</v>
       </c>
       <c r="E446" s="69" t="s">
         <v>2459</v>
@@ -19297,7 +19297,7 @@
         <v>2459</v>
       </c>
       <c r="D447" s="24" t="s">
-        <v>2633</v>
+        <v>2631</v>
       </c>
       <c r="E447" s="69" t="s">
         <v>2459</v>
@@ -19317,7 +19317,7 @@
         <v>2459</v>
       </c>
       <c r="D448" s="24" t="s">
-        <v>2634</v>
+        <v>2632</v>
       </c>
       <c r="E448" s="69" t="s">
         <v>2459</v>
@@ -19337,7 +19337,7 @@
         <v>2459</v>
       </c>
       <c r="D449" s="24" t="s">
-        <v>2635</v>
+        <v>2633</v>
       </c>
       <c r="E449" s="69" t="s">
         <v>2459</v>
@@ -19357,7 +19357,7 @@
         <v>2459</v>
       </c>
       <c r="D450" s="24" t="s">
-        <v>2636</v>
+        <v>2634</v>
       </c>
       <c r="E450" s="69" t="s">
         <v>2459</v>
@@ -19377,7 +19377,7 @@
         <v>2459</v>
       </c>
       <c r="D451" s="24" t="s">
-        <v>2637</v>
+        <v>2635</v>
       </c>
       <c r="E451" s="69" t="s">
         <v>2459</v>
@@ -19391,13 +19391,13 @@
         <v>2452</v>
       </c>
       <c r="B452" t="s">
-        <v>2638</v>
+        <v>2636</v>
       </c>
       <c r="C452" s="24" t="s">
         <v>1152</v>
       </c>
       <c r="D452" s="6" t="s">
-        <v>2639</v>
+        <v>2637</v>
       </c>
       <c r="E452" s="6" t="s">
         <v>1152</v>
@@ -19408,16 +19408,16 @@
     </row>
     <row r="453" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A453" s="6" t="s">
+        <v>2638</v>
+      </c>
+      <c r="B453" s="6" t="s">
+        <v>2639</v>
+      </c>
+      <c r="C453" s="24" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D453" s="6" t="s">
         <v>2640</v>
-      </c>
-      <c r="B453" s="6" t="s">
-        <v>2641</v>
-      </c>
-      <c r="C453" s="24" t="s">
-        <v>1152</v>
-      </c>
-      <c r="D453" s="6" t="s">
-        <v>2642</v>
       </c>
       <c r="E453" s="6" t="s">
         <v>1152</v>
@@ -22821,7 +22821,7 @@
   </sheetPr>
   <dimension ref="A1:V556"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A399" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D406" sqref="D406"/>
     </sheetView>
@@ -35483,7 +35483,7 @@
         <v>2452</v>
       </c>
       <c r="B546" s="70" t="s">
-        <v>2638</v>
+        <v>2636</v>
       </c>
       <c r="K546" s="70" t="s">
         <v>1323</v>
@@ -35617,10 +35617,10 @@
     </row>
     <row r="556" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A556" s="6" t="s">
-        <v>2640</v>
+        <v>2638</v>
       </c>
       <c r="B556" s="6" t="s">
-        <v>2643</v>
+        <v>2641</v>
       </c>
       <c r="K556" s="70" t="s">
         <v>1323</v>

</xml_diff>

<commit_message>
update marvl plot for field data
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/updates/tassielakes-data/data-governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0062E13D-8501-F142-9C43-B340ACB2CD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088FCCBF-4EB1-5B41-BB35-AD4009B5520A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9423,8 +9423,8 @@
   <dimension ref="A1:G453"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A341" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D362" sqref="D362"/>
+      <pane ySplit="1" topLeftCell="A409" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D421" sqref="D421"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Processed data and header csv files for cyanobacteria biomass; Update variable_key.xlsx, matfile and marvl plot for cyanobacteria biomass; upload marvl conversion information for phytoplankton biomass
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/updates/tassielakes-data/data-governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088FCCBF-4EB1-5B41-BB35-AD4009B5520A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BBE315-AE2C-744B-AA8E-DB42F8DCD289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,7 +434,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7219" uniqueCount="2644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7231" uniqueCount="2649">
   <si>
     <t>//</t>
   </si>
@@ -8492,6 +8492,21 @@
   </si>
   <si>
     <t>WQ_DIAG_PHY_GRN_ANKYRA</t>
+  </si>
+  <si>
+    <t>var00777</t>
+  </si>
+  <si>
+    <t>Phytoplankton Biomass (cyano)</t>
+  </si>
+  <si>
+    <t>PHY_{cyano}</t>
+  </si>
+  <si>
+    <t>phytoplankton_biomass_cyano</t>
+  </si>
+  <si>
+    <t>WQ_PHY_CYANO</t>
   </si>
 </sst>
 </file>
@@ -9420,11 +9435,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G453"/>
+  <dimension ref="A1:G454"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A409" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D421" sqref="D421"/>
+      <pane ySplit="1" topLeftCell="A433" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D456" sqref="D456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19423,6 +19438,27 @@
         <v>1152</v>
       </c>
       <c r="F453" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A454" s="6" t="s">
+        <v>2644</v>
+      </c>
+      <c r="B454" s="6" t="s">
+        <v>2645</v>
+      </c>
+      <c r="C454" s="40" t="str">
+        <f>VLOOKUP(A454,'MASTER KEY'!$A$2:$C1412,3,TRUE)</f>
+        <v>mmol C/m^3</v>
+      </c>
+      <c r="D454" s="27" t="s">
+        <v>2648</v>
+      </c>
+      <c r="E454" s="27" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F454" s="4">
         <v>1</v>
       </c>
     </row>
@@ -22819,11 +22855,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:V556"/>
+  <dimension ref="A1:V557"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A399" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D406" sqref="D406"/>
+      <pane ySplit="1" topLeftCell="A532" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B557" sqref="B557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35624,6 +35660,32 @@
       </c>
       <c r="K556" s="70" t="s">
         <v>1323</v>
+      </c>
+    </row>
+    <row r="557" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A557" s="6" t="s">
+        <v>2644</v>
+      </c>
+      <c r="B557" s="6" t="s">
+        <v>2645</v>
+      </c>
+      <c r="C557" s="2" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D557" s="2" t="s">
+        <v>2646</v>
+      </c>
+      <c r="E557" s="2" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F557" s="2" t="s">
+        <v>2647</v>
+      </c>
+      <c r="H557" s="2" t="s">
+        <v>1152</v>
+      </c>
+      <c r="K557" s="2" t="s">
+        <v>1456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update variable_key.xlsx, correlation between phycocyanin and cyanobacteria
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/updates/tassielakes-data/data-governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BBE315-AE2C-744B-AA8E-DB42F8DCD289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABF06D5-80BE-DF49-928A-EB06D474F07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8008,9 +8008,6 @@
     <t>WQ_GEO_CL</t>
   </si>
   <si>
-    <t>WQ_PHY_BGA</t>
-  </si>
-  <si>
     <t>WQ_GEO_FEII</t>
   </si>
   <si>
@@ -8507,6 +8504,9 @@
   </si>
   <si>
     <t>WQ_PHY_CYANO</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_CYANO</t>
   </si>
 </sst>
 </file>
@@ -9438,8 +9438,8 @@
   <dimension ref="A1:G454"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A433" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D456" sqref="D456"/>
+      <pane ySplit="1" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L315" sqref="L315:L319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10144,7 +10144,7 @@
         <v>mg/L</v>
       </c>
       <c r="D29" s="76" t="s">
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="E29" s="27" t="s">
         <v>1002</v>
@@ -12712,7 +12712,7 @@
         <v>m</v>
       </c>
       <c r="D136" s="27" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="E136" s="27" t="s">
         <v>1007</v>
@@ -13633,7 +13633,7 @@
         <v>µmol/m2/s</v>
       </c>
       <c r="D176" s="11" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="E176" s="27" t="s">
         <v>1152</v>
@@ -16686,7 +16686,7 @@
         <v>2459</v>
       </c>
       <c r="D316" s="5" t="s">
-        <v>2482</v>
+        <v>2648</v>
       </c>
       <c r="E316" t="s">
         <v>1002</v>
@@ -16706,7 +16706,7 @@
         <v>2457</v>
       </c>
       <c r="D317" s="5" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
       <c r="E317" t="s">
         <v>1002</v>
@@ -16726,7 +16726,7 @@
         <v>2457</v>
       </c>
       <c r="D318" s="5" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="E318" t="s">
         <v>1002</v>
@@ -16746,7 +16746,7 @@
         <v>2457</v>
       </c>
       <c r="D319" s="5" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
       <c r="E319" t="s">
         <v>1002</v>
@@ -16766,7 +16766,7 @@
         <v>2457</v>
       </c>
       <c r="D320" s="5" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="E320" t="s">
         <v>1002</v>
@@ -16786,7 +16786,7 @@
         <v>2463</v>
       </c>
       <c r="D321" s="5" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
       <c r="E321" t="s">
         <v>1002</v>
@@ -16806,7 +16806,7 @@
         <v>2463</v>
       </c>
       <c r="D322" s="5" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
       <c r="E322" t="s">
         <v>1002</v>
@@ -16847,7 +16847,7 @@
         <v>2457</v>
       </c>
       <c r="D324" s="5" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
       <c r="E324" t="s">
         <v>1002</v>
@@ -16868,7 +16868,7 @@
         <v>921</v>
       </c>
       <c r="D325" s="5" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
       <c r="E325" t="s">
         <v>1002</v>
@@ -16910,7 +16910,7 @@
         <v>2457</v>
       </c>
       <c r="D327" s="6" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
       <c r="E327" s="6" t="s">
         <v>1002</v>
@@ -16931,7 +16931,7 @@
         <v>2457</v>
       </c>
       <c r="D328" s="6" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
       <c r="E328" s="6" t="s">
         <v>1002</v>
@@ -16943,16 +16943,16 @@
     </row>
     <row r="329" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A329" s="75" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="B329" s="6" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="C329" s="69" t="s">
         <v>2459</v>
       </c>
       <c r="D329" s="6" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="E329" s="69" t="s">
         <v>2459</v>
@@ -16963,16 +16963,16 @@
     </row>
     <row r="330" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A330" s="75" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="B330" s="6" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="C330" s="69" t="s">
         <v>2459</v>
       </c>
       <c r="D330" s="6" t="s">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="E330" s="69" t="s">
         <v>2459</v>
@@ -16983,16 +16983,16 @@
     </row>
     <row r="331" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A331" s="75" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="B331" s="6" t="s">
-        <v>2513</v>
+        <v>2512</v>
       </c>
       <c r="C331" s="69" t="s">
         <v>2459</v>
       </c>
       <c r="D331" s="6" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="E331" s="69" t="s">
         <v>2459</v>
@@ -17003,16 +17003,16 @@
     </row>
     <row r="332" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A332" s="75" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="B332" s="6" t="s">
-        <v>2514</v>
+        <v>2513</v>
       </c>
       <c r="C332" s="69" t="s">
         <v>2459</v>
       </c>
       <c r="D332" s="6" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="E332" s="69" t="s">
         <v>2459</v>
@@ -17023,16 +17023,16 @@
     </row>
     <row r="333" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A333" s="75" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="B333" s="6" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
       <c r="C333" s="69" t="s">
         <v>2459</v>
       </c>
       <c r="D333" s="6" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="E333" s="69" t="s">
         <v>2459</v>
@@ -17043,16 +17043,16 @@
     </row>
     <row r="334" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A334" s="75" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
       <c r="B334" s="6" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
       <c r="C334" s="69" t="s">
         <v>2459</v>
       </c>
       <c r="D334" s="6" t="s">
-        <v>2506</v>
+        <v>2505</v>
       </c>
       <c r="E334" s="69" t="s">
         <v>2459</v>
@@ -17063,16 +17063,16 @@
     </row>
     <row r="335" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A335" s="75" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="B335" s="6" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="C335" s="69" t="s">
         <v>2459</v>
       </c>
       <c r="D335" s="6" t="s">
-        <v>2507</v>
+        <v>2506</v>
       </c>
       <c r="E335" s="69" t="s">
         <v>2459</v>
@@ -17083,16 +17083,16 @@
     </row>
     <row r="336" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A336" s="75" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
       <c r="B336" s="6" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="C336" s="69" t="s">
         <v>2459</v>
       </c>
       <c r="D336" s="6" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="E336" s="69" t="s">
         <v>2459</v>
@@ -17103,16 +17103,16 @@
     </row>
     <row r="337" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A337" s="75" t="s">
+        <v>2508</v>
+      </c>
+      <c r="B337" s="6" t="s">
+        <v>2518</v>
+      </c>
+      <c r="C337" s="69" t="s">
+        <v>2459</v>
+      </c>
+      <c r="D337" s="6" t="s">
         <v>2509</v>
-      </c>
-      <c r="B337" s="6" t="s">
-        <v>2519</v>
-      </c>
-      <c r="C337" s="69" t="s">
-        <v>2459</v>
-      </c>
-      <c r="D337" s="6" t="s">
-        <v>2510</v>
       </c>
       <c r="E337" s="69" t="s">
         <v>2459</v>
@@ -17132,7 +17132,7 @@
         <v>2459</v>
       </c>
       <c r="D338" s="24" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="E338" s="69" t="s">
         <v>2459</v>
@@ -17152,7 +17152,7 @@
         <v>2459</v>
       </c>
       <c r="D339" s="24" t="s">
-        <v>2524</v>
+        <v>2523</v>
       </c>
       <c r="E339" s="69" t="s">
         <v>2459</v>
@@ -17172,7 +17172,7 @@
         <v>2459</v>
       </c>
       <c r="D340" s="24" t="s">
-        <v>2525</v>
+        <v>2524</v>
       </c>
       <c r="E340" s="69" t="s">
         <v>2459</v>
@@ -17192,7 +17192,7 @@
         <v>2459</v>
       </c>
       <c r="D341" s="24" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
       <c r="E341" s="69" t="s">
         <v>2459</v>
@@ -17212,7 +17212,7 @@
         <v>2459</v>
       </c>
       <c r="D342" s="24" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
       <c r="E342" s="69" t="s">
         <v>2459</v>
@@ -17232,7 +17232,7 @@
         <v>2459</v>
       </c>
       <c r="D343" s="24" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
       <c r="E343" s="69" t="s">
         <v>2459</v>
@@ -17252,7 +17252,7 @@
         <v>2459</v>
       </c>
       <c r="D344" s="24" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="E344" s="69" t="s">
         <v>2459</v>
@@ -17272,7 +17272,7 @@
         <v>2459</v>
       </c>
       <c r="D345" s="24" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="E345" s="69" t="s">
         <v>2459</v>
@@ -17292,7 +17292,7 @@
         <v>2459</v>
       </c>
       <c r="D346" s="24" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="E346" s="69" t="s">
         <v>2459</v>
@@ -17312,7 +17312,7 @@
         <v>2459</v>
       </c>
       <c r="D347" s="24" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
       <c r="E347" s="69" t="s">
         <v>2459</v>
@@ -17332,7 +17332,7 @@
         <v>2459</v>
       </c>
       <c r="D348" s="24" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
       <c r="E348" s="69" t="s">
         <v>2459</v>
@@ -17352,7 +17352,7 @@
         <v>2459</v>
       </c>
       <c r="D349" s="24" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
       <c r="E349" s="69" t="s">
         <v>2459</v>
@@ -17372,7 +17372,7 @@
         <v>2459</v>
       </c>
       <c r="D350" s="24" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="E350" s="69" t="s">
         <v>2459</v>
@@ -17392,7 +17392,7 @@
         <v>2459</v>
       </c>
       <c r="D351" s="24" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="E351" s="69" t="s">
         <v>2459</v>
@@ -17412,7 +17412,7 @@
         <v>2459</v>
       </c>
       <c r="D352" s="24" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="E352" s="69" t="s">
         <v>2459</v>
@@ -17432,7 +17432,7 @@
         <v>2459</v>
       </c>
       <c r="D353" s="24" t="s">
-        <v>2538</v>
+        <v>2537</v>
       </c>
       <c r="E353" s="69" t="s">
         <v>2459</v>
@@ -17452,7 +17452,7 @@
         <v>2459</v>
       </c>
       <c r="D354" s="24" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="E354" s="69" t="s">
         <v>2459</v>
@@ -17472,7 +17472,7 @@
         <v>2459</v>
       </c>
       <c r="D355" s="24" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="E355" s="69" t="s">
         <v>2459</v>
@@ -17492,7 +17492,7 @@
         <v>2459</v>
       </c>
       <c r="D356" s="24" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="E356" s="69" t="s">
         <v>2459</v>
@@ -17512,7 +17512,7 @@
         <v>2459</v>
       </c>
       <c r="D357" s="24" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="E357" s="69" t="s">
         <v>2459</v>
@@ -17532,7 +17532,7 @@
         <v>2459</v>
       </c>
       <c r="D358" s="24" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="E358" s="69" t="s">
         <v>2459</v>
@@ -17552,7 +17552,7 @@
         <v>2459</v>
       </c>
       <c r="D359" s="24" t="s">
-        <v>2544</v>
+        <v>2543</v>
       </c>
       <c r="E359" s="69" t="s">
         <v>2459</v>
@@ -17572,7 +17572,7 @@
         <v>2459</v>
       </c>
       <c r="D360" s="24" t="s">
-        <v>2545</v>
+        <v>2544</v>
       </c>
       <c r="E360" s="69" t="s">
         <v>2459</v>
@@ -17592,7 +17592,7 @@
         <v>2459</v>
       </c>
       <c r="D361" s="24" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
       <c r="E361" s="69" t="s">
         <v>2459</v>
@@ -17612,7 +17612,7 @@
         <v>2459</v>
       </c>
       <c r="D362" s="24" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
       <c r="E362" s="69" t="s">
         <v>2459</v>
@@ -17632,7 +17632,7 @@
         <v>2459</v>
       </c>
       <c r="D363" s="24" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="E363" s="69" t="s">
         <v>2459</v>
@@ -17652,7 +17652,7 @@
         <v>2459</v>
       </c>
       <c r="D364" s="24" t="s">
-        <v>2547</v>
+        <v>2546</v>
       </c>
       <c r="E364" s="69" t="s">
         <v>2459</v>
@@ -17672,7 +17672,7 @@
         <v>2459</v>
       </c>
       <c r="D365" s="24" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
       <c r="E365" s="69" t="s">
         <v>2459</v>
@@ -17692,7 +17692,7 @@
         <v>2459</v>
       </c>
       <c r="D366" s="24" t="s">
-        <v>2549</v>
+        <v>2548</v>
       </c>
       <c r="E366" s="69" t="s">
         <v>2459</v>
@@ -17712,7 +17712,7 @@
         <v>2459</v>
       </c>
       <c r="D367" s="24" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="E367" s="69" t="s">
         <v>2459</v>
@@ -17732,7 +17732,7 @@
         <v>2459</v>
       </c>
       <c r="D368" s="24" t="s">
-        <v>2551</v>
+        <v>2550</v>
       </c>
       <c r="E368" s="69" t="s">
         <v>2459</v>
@@ -17752,7 +17752,7 @@
         <v>2459</v>
       </c>
       <c r="D369" s="24" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="E369" s="69" t="s">
         <v>2459</v>
@@ -17772,7 +17772,7 @@
         <v>2459</v>
       </c>
       <c r="D370" s="24" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="E370" s="69" t="s">
         <v>2459</v>
@@ -17792,7 +17792,7 @@
         <v>2459</v>
       </c>
       <c r="D371" s="24" t="s">
-        <v>2554</v>
+        <v>2553</v>
       </c>
       <c r="E371" s="69" t="s">
         <v>2459</v>
@@ -17812,7 +17812,7 @@
         <v>2459</v>
       </c>
       <c r="D372" s="24" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="E372" s="69" t="s">
         <v>2459</v>
@@ -17832,7 +17832,7 @@
         <v>2459</v>
       </c>
       <c r="D373" s="24" t="s">
-        <v>2556</v>
+        <v>2555</v>
       </c>
       <c r="E373" s="69" t="s">
         <v>2459</v>
@@ -17852,7 +17852,7 @@
         <v>2459</v>
       </c>
       <c r="D374" s="24" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E374" s="69" t="s">
         <v>2459</v>
@@ -17872,7 +17872,7 @@
         <v>2459</v>
       </c>
       <c r="D375" s="24" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="E375" s="69" t="s">
         <v>2459</v>
@@ -17892,7 +17892,7 @@
         <v>2459</v>
       </c>
       <c r="D376" s="24" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="E376" s="69" t="s">
         <v>2459</v>
@@ -17912,7 +17912,7 @@
         <v>2459</v>
       </c>
       <c r="D377" s="24" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="E377" s="69" t="s">
         <v>2459</v>
@@ -17932,7 +17932,7 @@
         <v>2459</v>
       </c>
       <c r="D378" s="24" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="E378" s="69" t="s">
         <v>2459</v>
@@ -17952,7 +17952,7 @@
         <v>2459</v>
       </c>
       <c r="D379" s="24" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
       <c r="E379" s="69" t="s">
         <v>2459</v>
@@ -17972,7 +17972,7 @@
         <v>2459</v>
       </c>
       <c r="D380" s="24" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="E380" s="69" t="s">
         <v>2459</v>
@@ -17992,7 +17992,7 @@
         <v>2459</v>
       </c>
       <c r="D381" s="24" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
       <c r="E381" s="69" t="s">
         <v>2459</v>
@@ -18012,7 +18012,7 @@
         <v>2459</v>
       </c>
       <c r="D382" s="24" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="E382" s="69" t="s">
         <v>2459</v>
@@ -18032,7 +18032,7 @@
         <v>2459</v>
       </c>
       <c r="D383" s="24" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="E383" s="69" t="s">
         <v>2459</v>
@@ -18052,7 +18052,7 @@
         <v>2459</v>
       </c>
       <c r="D384" s="24" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="E384" s="69" t="s">
         <v>2459</v>
@@ -18072,7 +18072,7 @@
         <v>2459</v>
       </c>
       <c r="D385" s="24" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="E385" s="69" t="s">
         <v>2459</v>
@@ -18092,7 +18092,7 @@
         <v>2459</v>
       </c>
       <c r="D386" s="24" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
       <c r="E386" s="69" t="s">
         <v>2459</v>
@@ -18112,7 +18112,7 @@
         <v>2459</v>
       </c>
       <c r="D387" s="24" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="E387" s="69" t="s">
         <v>2459</v>
@@ -18132,7 +18132,7 @@
         <v>2459</v>
       </c>
       <c r="D388" s="24" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
       <c r="E388" s="69" t="s">
         <v>2459</v>
@@ -18152,7 +18152,7 @@
         <v>2459</v>
       </c>
       <c r="D389" s="24" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="E389" s="69" t="s">
         <v>2459</v>
@@ -18172,7 +18172,7 @@
         <v>2459</v>
       </c>
       <c r="D390" s="24" t="s">
-        <v>2573</v>
+        <v>2572</v>
       </c>
       <c r="E390" s="69" t="s">
         <v>2459</v>
@@ -18192,7 +18192,7 @@
         <v>2459</v>
       </c>
       <c r="D391" s="24" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="E391" s="69" t="s">
         <v>2459</v>
@@ -18212,7 +18212,7 @@
         <v>2459</v>
       </c>
       <c r="D392" s="24" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="E392" s="69" t="s">
         <v>2459</v>
@@ -18232,7 +18232,7 @@
         <v>2459</v>
       </c>
       <c r="D393" s="24" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
       <c r="E393" s="69" t="s">
         <v>2459</v>
@@ -18252,7 +18252,7 @@
         <v>2459</v>
       </c>
       <c r="D394" s="24" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="E394" s="69" t="s">
         <v>2459</v>
@@ -18272,7 +18272,7 @@
         <v>2459</v>
       </c>
       <c r="D395" s="24" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
       <c r="E395" s="69" t="s">
         <v>2459</v>
@@ -18292,7 +18292,7 @@
         <v>2459</v>
       </c>
       <c r="D396" s="24" t="s">
-        <v>2579</v>
+        <v>2578</v>
       </c>
       <c r="E396" s="69" t="s">
         <v>2459</v>
@@ -18312,7 +18312,7 @@
         <v>2459</v>
       </c>
       <c r="D397" s="24" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="E397" s="69" t="s">
         <v>2459</v>
@@ -18332,7 +18332,7 @@
         <v>2459</v>
       </c>
       <c r="D398" s="24" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
       <c r="E398" s="69" t="s">
         <v>2459</v>
@@ -18352,7 +18352,7 @@
         <v>2459</v>
       </c>
       <c r="D399" s="24" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="E399" s="69" t="s">
         <v>2459</v>
@@ -18372,7 +18372,7 @@
         <v>2459</v>
       </c>
       <c r="D400" s="24" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
       <c r="E400" s="69" t="s">
         <v>2459</v>
@@ -18392,7 +18392,7 @@
         <v>2459</v>
       </c>
       <c r="D401" s="24" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="E401" s="69" t="s">
         <v>2459</v>
@@ -18412,7 +18412,7 @@
         <v>2459</v>
       </c>
       <c r="D402" s="24" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
       <c r="E402" s="69" t="s">
         <v>2459</v>
@@ -18432,7 +18432,7 @@
         <v>2459</v>
       </c>
       <c r="D403" s="24" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
       <c r="E403" s="69" t="s">
         <v>2459</v>
@@ -18452,7 +18452,7 @@
         <v>2459</v>
       </c>
       <c r="D404" s="24" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
       <c r="E404" s="69" t="s">
         <v>2459</v>
@@ -18472,7 +18472,7 @@
         <v>2459</v>
       </c>
       <c r="D405" s="24" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="E405" s="69" t="s">
         <v>2459</v>
@@ -18492,7 +18492,7 @@
         <v>2459</v>
       </c>
       <c r="D406" s="24" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="E406" s="69" t="s">
         <v>2459</v>
@@ -18512,7 +18512,7 @@
         <v>2459</v>
       </c>
       <c r="D407" s="24" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
       <c r="E407" s="69" t="s">
         <v>2459</v>
@@ -18532,7 +18532,7 @@
         <v>2459</v>
       </c>
       <c r="D408" s="24" t="s">
-        <v>2591</v>
+        <v>2590</v>
       </c>
       <c r="E408" s="69" t="s">
         <v>2459</v>
@@ -18552,7 +18552,7 @@
         <v>2459</v>
       </c>
       <c r="D409" s="24" t="s">
-        <v>2592</v>
+        <v>2591</v>
       </c>
       <c r="E409" s="69" t="s">
         <v>2459</v>
@@ -18572,7 +18572,7 @@
         <v>2459</v>
       </c>
       <c r="D410" s="24" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
       <c r="E410" s="69" t="s">
         <v>2459</v>
@@ -18592,7 +18592,7 @@
         <v>2459</v>
       </c>
       <c r="D411" s="24" t="s">
-        <v>2594</v>
+        <v>2593</v>
       </c>
       <c r="E411" s="69" t="s">
         <v>2459</v>
@@ -18612,7 +18612,7 @@
         <v>2459</v>
       </c>
       <c r="D412" s="24" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="E412" s="69" t="s">
         <v>2459</v>
@@ -18632,7 +18632,7 @@
         <v>2459</v>
       </c>
       <c r="D413" s="24" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
       <c r="E413" s="69" t="s">
         <v>2459</v>
@@ -18652,7 +18652,7 @@
         <v>2459</v>
       </c>
       <c r="D414" s="24" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
       <c r="E414" s="69" t="s">
         <v>2459</v>
@@ -18672,7 +18672,7 @@
         <v>2459</v>
       </c>
       <c r="D415" s="24" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="E415" s="69" t="s">
         <v>2459</v>
@@ -18692,7 +18692,7 @@
         <v>2459</v>
       </c>
       <c r="D416" s="24" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
       <c r="E416" s="69" t="s">
         <v>2459</v>
@@ -18712,7 +18712,7 @@
         <v>2459</v>
       </c>
       <c r="D417" s="24" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="E417" s="69" t="s">
         <v>2459</v>
@@ -18732,7 +18732,7 @@
         <v>2459</v>
       </c>
       <c r="D418" s="24" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="E418" s="69" t="s">
         <v>2459</v>
@@ -18752,7 +18752,7 @@
         <v>2459</v>
       </c>
       <c r="D419" s="24" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="E419" s="69" t="s">
         <v>2459</v>
@@ -18772,7 +18772,7 @@
         <v>2459</v>
       </c>
       <c r="D420" s="24" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="E420" s="69" t="s">
         <v>2459</v>
@@ -18792,7 +18792,7 @@
         <v>2459</v>
       </c>
       <c r="D421" s="24" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="E421" s="69" t="s">
         <v>2459</v>
@@ -18812,7 +18812,7 @@
         <v>2459</v>
       </c>
       <c r="D422" s="24" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
       <c r="E422" s="69" t="s">
         <v>2459</v>
@@ -18832,7 +18832,7 @@
         <v>2459</v>
       </c>
       <c r="D423" s="24" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
       <c r="E423" s="69" t="s">
         <v>2459</v>
@@ -18852,7 +18852,7 @@
         <v>2459</v>
       </c>
       <c r="D424" s="24" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
       <c r="E424" s="69" t="s">
         <v>2459</v>
@@ -18866,13 +18866,13 @@
         <v>2329</v>
       </c>
       <c r="B425" t="s">
+        <v>2607</v>
+      </c>
+      <c r="C425" s="69" t="s">
+        <v>2459</v>
+      </c>
+      <c r="D425" s="24" t="s">
         <v>2608</v>
-      </c>
-      <c r="C425" s="69" t="s">
-        <v>2459</v>
-      </c>
-      <c r="D425" s="24" t="s">
-        <v>2609</v>
       </c>
       <c r="E425" s="69" t="s">
         <v>2459</v>
@@ -18892,7 +18892,7 @@
         <v>2459</v>
       </c>
       <c r="D426" s="24" t="s">
-        <v>2610</v>
+        <v>2609</v>
       </c>
       <c r="E426" s="69" t="s">
         <v>2459</v>
@@ -18912,7 +18912,7 @@
         <v>2459</v>
       </c>
       <c r="D427" s="24" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
       <c r="E427" s="69" t="s">
         <v>2459</v>
@@ -18932,7 +18932,7 @@
         <v>2459</v>
       </c>
       <c r="D428" s="24" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
       <c r="E428" s="69" t="s">
         <v>2459</v>
@@ -18952,7 +18952,7 @@
         <v>2459</v>
       </c>
       <c r="D429" s="24" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="E429" s="69" t="s">
         <v>2459</v>
@@ -18972,7 +18972,7 @@
         <v>2459</v>
       </c>
       <c r="D430" s="24" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
       <c r="E430" s="69" t="s">
         <v>2459</v>
@@ -18992,7 +18992,7 @@
         <v>2459</v>
       </c>
       <c r="D431" s="24" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
       <c r="E431" s="69" t="s">
         <v>2459</v>
@@ -19012,7 +19012,7 @@
         <v>2459</v>
       </c>
       <c r="D432" s="24" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
       <c r="E432" s="69" t="s">
         <v>2459</v>
@@ -19032,7 +19032,7 @@
         <v>2459</v>
       </c>
       <c r="D433" s="24" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
       <c r="E433" s="69" t="s">
         <v>2459</v>
@@ -19052,7 +19052,7 @@
         <v>2459</v>
       </c>
       <c r="D434" s="24" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
       <c r="E434" s="69" t="s">
         <v>2459</v>
@@ -19072,7 +19072,7 @@
         <v>2459</v>
       </c>
       <c r="D435" s="24" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
       <c r="E435" s="69" t="s">
         <v>2459</v>
@@ -19092,7 +19092,7 @@
         <v>2459</v>
       </c>
       <c r="D436" s="24" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
       <c r="E436" s="69" t="s">
         <v>2459</v>
@@ -19112,7 +19112,7 @@
         <v>2459</v>
       </c>
       <c r="D437" s="24" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="E437" s="69" t="s">
         <v>2459</v>
@@ -19132,7 +19132,7 @@
         <v>2459</v>
       </c>
       <c r="D438" s="24" t="s">
-        <v>2622</v>
+        <v>2621</v>
       </c>
       <c r="E438" s="69" t="s">
         <v>2459</v>
@@ -19152,7 +19152,7 @@
         <v>2459</v>
       </c>
       <c r="D439" s="24" t="s">
-        <v>2623</v>
+        <v>2622</v>
       </c>
       <c r="E439" s="69" t="s">
         <v>2459</v>
@@ -19172,7 +19172,7 @@
         <v>2459</v>
       </c>
       <c r="D440" s="24" t="s">
-        <v>2624</v>
+        <v>2623</v>
       </c>
       <c r="E440" s="69" t="s">
         <v>2459</v>
@@ -19192,7 +19192,7 @@
         <v>2459</v>
       </c>
       <c r="D441" s="24" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
       <c r="E441" s="69" t="s">
         <v>2459</v>
@@ -19212,7 +19212,7 @@
         <v>2459</v>
       </c>
       <c r="D442" s="24" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
       <c r="E442" s="69" t="s">
         <v>2459</v>
@@ -19232,7 +19232,7 @@
         <v>2459</v>
       </c>
       <c r="D443" s="24" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
       <c r="E443" s="69" t="s">
         <v>2459</v>
@@ -19252,7 +19252,7 @@
         <v>2459</v>
       </c>
       <c r="D444" s="24" t="s">
-        <v>2628</v>
+        <v>2627</v>
       </c>
       <c r="E444" s="69" t="s">
         <v>2459</v>
@@ -19272,7 +19272,7 @@
         <v>2459</v>
       </c>
       <c r="D445" s="24" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
       <c r="E445" s="69" t="s">
         <v>2459</v>
@@ -19292,7 +19292,7 @@
         <v>2459</v>
       </c>
       <c r="D446" s="24" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
       <c r="E446" s="69" t="s">
         <v>2459</v>
@@ -19312,7 +19312,7 @@
         <v>2459</v>
       </c>
       <c r="D447" s="24" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
       <c r="E447" s="69" t="s">
         <v>2459</v>
@@ -19332,7 +19332,7 @@
         <v>2459</v>
       </c>
       <c r="D448" s="24" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
       <c r="E448" s="69" t="s">
         <v>2459</v>
@@ -19352,7 +19352,7 @@
         <v>2459</v>
       </c>
       <c r="D449" s="24" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="E449" s="69" t="s">
         <v>2459</v>
@@ -19372,7 +19372,7 @@
         <v>2459</v>
       </c>
       <c r="D450" s="24" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
       <c r="E450" s="69" t="s">
         <v>2459</v>
@@ -19392,7 +19392,7 @@
         <v>2459</v>
       </c>
       <c r="D451" s="24" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="E451" s="69" t="s">
         <v>2459</v>
@@ -19406,13 +19406,13 @@
         <v>2452</v>
       </c>
       <c r="B452" t="s">
+        <v>2635</v>
+      </c>
+      <c r="C452" s="24" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D452" s="6" t="s">
         <v>2636</v>
-      </c>
-      <c r="C452" s="24" t="s">
-        <v>1152</v>
-      </c>
-      <c r="D452" s="6" t="s">
-        <v>2637</v>
       </c>
       <c r="E452" s="6" t="s">
         <v>1152</v>
@@ -19423,16 +19423,16 @@
     </row>
     <row r="453" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A453" s="6" t="s">
+        <v>2637</v>
+      </c>
+      <c r="B453" s="6" t="s">
         <v>2638</v>
       </c>
-      <c r="B453" s="6" t="s">
+      <c r="C453" s="24" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D453" s="6" t="s">
         <v>2639</v>
-      </c>
-      <c r="C453" s="24" t="s">
-        <v>1152</v>
-      </c>
-      <c r="D453" s="6" t="s">
-        <v>2640</v>
       </c>
       <c r="E453" s="6" t="s">
         <v>1152</v>
@@ -19443,17 +19443,17 @@
     </row>
     <row r="454" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A454" s="6" t="s">
+        <v>2643</v>
+      </c>
+      <c r="B454" s="6" t="s">
         <v>2644</v>
-      </c>
-      <c r="B454" s="6" t="s">
-        <v>2645</v>
       </c>
       <c r="C454" s="40" t="str">
         <f>VLOOKUP(A454,'MASTER KEY'!$A$2:$C1412,3,TRUE)</f>
         <v>mmol C/m^3</v>
       </c>
       <c r="D454" s="27" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
       <c r="E454" s="27" t="s">
         <v>1041</v>
@@ -35519,7 +35519,7 @@
         <v>2452</v>
       </c>
       <c r="B546" s="70" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="K546" s="70" t="s">
         <v>1323</v>
@@ -35527,10 +35527,10 @@
     </row>
     <row r="547" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A547" s="69" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="B547" s="6" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="C547" s="69" t="s">
         <v>2459</v>
@@ -35541,10 +35541,10 @@
     </row>
     <row r="548" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A548" s="69" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="B548" s="6" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="C548" s="69" t="s">
         <v>2459</v>
@@ -35555,10 +35555,10 @@
     </row>
     <row r="549" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A549" s="69" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="B549" s="6" t="s">
-        <v>2513</v>
+        <v>2512</v>
       </c>
       <c r="C549" s="69" t="s">
         <v>2459</v>
@@ -35569,10 +35569,10 @@
     </row>
     <row r="550" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A550" s="69" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="B550" s="6" t="s">
-        <v>2514</v>
+        <v>2513</v>
       </c>
       <c r="C550" s="69" t="s">
         <v>2459</v>
@@ -35583,10 +35583,10 @@
     </row>
     <row r="551" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A551" s="69" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="B551" s="6" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
       <c r="C551" s="69" t="s">
         <v>2459</v>
@@ -35597,10 +35597,10 @@
     </row>
     <row r="552" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A552" s="69" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
       <c r="B552" s="6" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
       <c r="C552" s="69" t="s">
         <v>2459</v>
@@ -35611,10 +35611,10 @@
     </row>
     <row r="553" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A553" s="69" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="B553" s="6" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="C553" s="69" t="s">
         <v>2459</v>
@@ -35625,10 +35625,10 @@
     </row>
     <row r="554" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A554" s="69" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
       <c r="B554" s="6" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="C554" s="69" t="s">
         <v>2459</v>
@@ -35639,10 +35639,10 @@
     </row>
     <row r="555" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A555" s="6" t="s">
-        <v>2509</v>
+        <v>2508</v>
       </c>
       <c r="B555" s="6" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="C555" s="6" t="s">
         <v>2459</v>
@@ -35653,10 +35653,10 @@
     </row>
     <row r="556" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A556" s="6" t="s">
-        <v>2638</v>
+        <v>2637</v>
       </c>
       <c r="B556" s="6" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="K556" s="70" t="s">
         <v>1323</v>
@@ -35664,22 +35664,22 @@
     </row>
     <row r="557" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A557" s="6" t="s">
+        <v>2643</v>
+      </c>
+      <c r="B557" s="6" t="s">
         <v>2644</v>
-      </c>
-      <c r="B557" s="6" t="s">
-        <v>2645</v>
       </c>
       <c r="C557" s="2" t="s">
         <v>1041</v>
       </c>
       <c r="D557" s="2" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="E557" s="2" t="s">
         <v>1041</v>
       </c>
       <c r="F557" s="2" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
       <c r="H557" s="2" t="s">
         <v>1152</v>

</xml_diff>

<commit_message>
update variable key total alkalinity tfv conversion factor
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/tassielakes-data/data-governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F0405F-2A74-744C-B56C-69CB3CA5DAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5546304F-D52E-0945-9DC2-804AA323C278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="-17200" windowWidth="29400" windowHeight="17200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -36952,8 +36952,8 @@
   <dimension ref="A1:G487"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A464" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D486" sqref="D486"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F135" sqref="F135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40186,7 +40186,8 @@
         <v>1002</v>
       </c>
       <c r="F134" s="41">
-        <v>100.0869</v>
+        <f>1000/100.9</f>
+        <v>9.9108027750247771</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>